<commit_message>
Added 50 labels; Total 100
</commit_message>
<xml_diff>
--- a/John.xlsx
+++ b/John.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d03dc4ea78fd367a/Documents/S. Y. 2021-2022/1st Sem/Senior Thesis/data labeling/Final data labeling/data-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73F5745A-2714-420D-843C-3A200332528B}"/>
+  <xr:revisionPtr revIDLastSave="238" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C28CCE92-F283-44A4-ADF1-74079C5A4030}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="3705" windowWidth="21600" windowHeight="11385" xr2:uid="{77CB7C1E-B4AD-45B5-9992-3E1454331525}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Filename</t>
   </si>
@@ -223,6 +223,156 @@
   </si>
   <si>
     <t>DirectoryFactory.java</t>
+  </si>
+  <si>
+    <t>DirectoryImpl.java</t>
+  </si>
+  <si>
+    <t>DivisionMethod.java</t>
+  </si>
+  <si>
+    <t>double_hash (2).py</t>
+  </si>
+  <si>
+    <t>double_hash (3).py</t>
+  </si>
+  <si>
+    <t>double_hash (4).py</t>
+  </si>
+  <si>
+    <t>double_hash.py</t>
+  </si>
+  <si>
+    <t>double_hashing.py</t>
+  </si>
+  <si>
+    <t>DoubleHashing.java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList.java</t>
+  </si>
+  <si>
+    <t>Driver.java</t>
+  </si>
+  <si>
+    <t>dynamic_hashing.py</t>
+  </si>
+  <si>
+    <t>Entry.java</t>
+  </si>
+  <si>
+    <t>EntryIterator.java</t>
+  </si>
+  <si>
+    <t>EntrySet.java</t>
+  </si>
+  <si>
+    <t>FastMap.java</t>
+  </si>
+  <si>
+    <t>first-recurring-number.js</t>
+  </si>
+  <si>
+    <t>FixedSizedHashMap.java</t>
+  </si>
+  <si>
+    <t>hash_table (2).py</t>
+  </si>
+  <si>
+    <t>hash_table (3).py</t>
+  </si>
+  <si>
+    <t>hash_table (4).py</t>
+  </si>
+  <si>
+    <t>hash_table (5).py</t>
+  </si>
+  <si>
+    <t>hash_table_with_linked_list (2).py</t>
+  </si>
+  <si>
+    <t>hash_table_with_linked_list (3).py</t>
+  </si>
+  <si>
+    <t>hash_table_with_linked_list (4).py</t>
+  </si>
+  <si>
+    <t>hash_table_with_linked_list.py</t>
+  </si>
+  <si>
+    <t>hash_table.py</t>
+  </si>
+  <si>
+    <t>hash-table.js</t>
+  </si>
+  <si>
+    <t>Hash.js</t>
+  </si>
+  <si>
+    <t>HashArrayMappedTrie.java</t>
+  </si>
+  <si>
+    <t>HashCodeAndEquals.java</t>
+  </si>
+  <si>
+    <t>HashEntry.java</t>
+  </si>
+  <si>
+    <t>HashFunction (2).java</t>
+  </si>
+  <si>
+    <t>HashFunction.java</t>
+  </si>
+  <si>
+    <t>HashMap (2).java</t>
+  </si>
+  <si>
+    <t>HashMap (3).java</t>
+  </si>
+  <si>
+    <t>HashMap (4).java</t>
+  </si>
+  <si>
+    <t>HashMap (5).java</t>
+  </si>
+  <si>
+    <t>HashMap (6).java</t>
+  </si>
+  <si>
+    <t>HashMap (7).java</t>
+  </si>
+  <si>
+    <t>HashMap (8).java</t>
+  </si>
+  <si>
+    <t>HashMap (9).java</t>
+  </si>
+  <si>
+    <t>HashMap (10).java</t>
+  </si>
+  <si>
+    <t>HashMap (11).java</t>
+  </si>
+  <si>
+    <t>HashMap (12).java</t>
+  </si>
+  <si>
+    <t>HashMap (13).java</t>
+  </si>
+  <si>
+    <t>HashMap (14).java</t>
+  </si>
+  <si>
+    <t>HashMap.java</t>
+  </si>
+  <si>
+    <t>HashMap.js</t>
+  </si>
+  <si>
+    <t>hashmap.py</t>
+  </si>
+  <si>
+    <t>HashMapDriver.java</t>
   </si>
 </sst>
 </file>
@@ -595,11 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E621E51-50FD-4EF4-866F-BB44D85D3FB2}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,6 +2411,1606 @@
         <v>0</v>
       </c>
     </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>107</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>112</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done labeling contents of Hash-Map folder; Total: 218
</commit_message>
<xml_diff>
--- a/John.xlsx
+++ b/John.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d03dc4ea78fd367a/Documents/S. Y. 2021-2022/1st Sem/Senior Thesis/data labeling/Final data labeling/data-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="238" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C28CCE92-F283-44A4-ADF1-74079C5A4030}"/>
+  <xr:revisionPtr revIDLastSave="534" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E371093B-E5D6-4A54-B7A5-1AAF51972A38}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="3705" windowWidth="21600" windowHeight="11385" xr2:uid="{77CB7C1E-B4AD-45B5-9992-3E1454331525}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
   <si>
     <t>Filename</t>
   </si>
@@ -373,6 +373,360 @@
   </si>
   <si>
     <t>HashMapDriver.java</t>
+  </si>
+  <si>
+    <t>HashMapEntry.java</t>
+  </si>
+  <si>
+    <t>HashMapImplementation.java</t>
+  </si>
+  <si>
+    <t>HashMapInterface (2).java</t>
+  </si>
+  <si>
+    <t>HashMapInterface (3).java</t>
+  </si>
+  <si>
+    <t>HashMapInterface.java</t>
+  </si>
+  <si>
+    <t>HashMapSeparateChaining.java</t>
+  </si>
+  <si>
+    <t>HashMapX.java</t>
+  </si>
+  <si>
+    <t>HashSequence.java</t>
+  </si>
+  <si>
+    <t>HashStrategy.java</t>
+  </si>
+  <si>
+    <t>HashTable.java</t>
+  </si>
+  <si>
+    <t>HashTableChaining.java</t>
+  </si>
+  <si>
+    <t>HashTableOpenAddressing.java</t>
+  </si>
+  <si>
+    <t>HashTester (2).java</t>
+  </si>
+  <si>
+    <t>HashTester.java</t>
+  </si>
+  <si>
+    <t>implementing-hash-table.js</t>
+  </si>
+  <si>
+    <t>ImplicitKeyTreap.java</t>
+  </si>
+  <si>
+    <t>JavaSerializer.java</t>
+  </si>
+  <si>
+    <t>Key.java</t>
+  </si>
+  <si>
+    <t>KeyedObjectFactory.js</t>
+  </si>
+  <si>
+    <t>KeyIterator.java</t>
+  </si>
+  <si>
+    <t>KeyNotFoundException.java</t>
+  </si>
+  <si>
+    <t>KeySet.java</t>
+  </si>
+  <si>
+    <t>KeyValueNode.java</t>
+  </si>
+  <si>
+    <t>KeyValuePair.java</t>
+  </si>
+  <si>
+    <t>KeyValuePojo.java</t>
+  </si>
+  <si>
+    <t>KpcbHash.java</t>
+  </si>
+  <si>
+    <t>LazyStudent (2).java</t>
+  </si>
+  <si>
+    <t>LazyStudent.java</t>
+  </si>
+  <si>
+    <t>linearmap.py</t>
+  </si>
+  <si>
+    <t>LinearProbing.java</t>
+  </si>
+  <si>
+    <t>LinearProbingBucketImpl.java</t>
+  </si>
+  <si>
+    <t>LinkedList (2).java</t>
+  </si>
+  <si>
+    <t>LinkedList (3).java</t>
+  </si>
+  <si>
+    <t>LinkedList (4).java</t>
+  </si>
+  <si>
+    <t>LinkedList.java</t>
+  </si>
+  <si>
+    <t>LRUCache.java</t>
+  </si>
+  <si>
+    <t>LRUCache.js</t>
+  </si>
+  <si>
+    <t>Main (2).java</t>
+  </si>
+  <si>
+    <t>Main (3).java</t>
+  </si>
+  <si>
+    <t>Main (4).java</t>
+  </si>
+  <si>
+    <t>Main (5).java</t>
+  </si>
+  <si>
+    <t>Main (6).java</t>
+  </si>
+  <si>
+    <t>Main (7).java</t>
+  </si>
+  <si>
+    <t>Main (8).java</t>
+  </si>
+  <si>
+    <t>Main (9).java</t>
+  </si>
+  <si>
+    <t>Main (10).java</t>
+  </si>
+  <si>
+    <t>Main (11).java</t>
+  </si>
+  <si>
+    <t>Main.java</t>
+  </si>
+  <si>
+    <t>MainClass (2).java</t>
+  </si>
+  <si>
+    <t>MainClass.java</t>
+  </si>
+  <si>
+    <t>Map (2).java</t>
+  </si>
+  <si>
+    <t>Map.java</t>
+  </si>
+  <si>
+    <t>Map.js</t>
+  </si>
+  <si>
+    <t>MapEntry (2).java</t>
+  </si>
+  <si>
+    <t>MapEntry (3).java</t>
+  </si>
+  <si>
+    <t>MapEntry (4).java</t>
+  </si>
+  <si>
+    <t>MapEntry.java</t>
+  </si>
+  <si>
+    <t>MathGeneral.java</t>
+  </si>
+  <si>
+    <t>MetricsSupport.java</t>
+  </si>
+  <si>
+    <t>MultiplicationMethod.java</t>
+  </si>
+  <si>
+    <t>MultiStringColl.java</t>
+  </si>
+  <si>
+    <t>MultiStringCollClient.java</t>
+  </si>
+  <si>
+    <t>MyHashMap (2).java</t>
+  </si>
+  <si>
+    <t>MyHashMap (3).java</t>
+  </si>
+  <si>
+    <t>MyHashMap.java</t>
+  </si>
+  <si>
+    <t>MyHashMapImpl (2).java</t>
+  </si>
+  <si>
+    <t>MyHashMapImpl.java</t>
+  </si>
+  <si>
+    <t>Nashmap.java</t>
+  </si>
+  <si>
+    <t>NeedExpansionException.java</t>
+  </si>
+  <si>
+    <t>Node (2).java</t>
+  </si>
+  <si>
+    <t>Node (3).java</t>
+  </si>
+  <si>
+    <t>Node (4).java</t>
+  </si>
+  <si>
+    <t>Node (5).java</t>
+  </si>
+  <si>
+    <t>Node.java</t>
+  </si>
+  <si>
+    <t>ObjectCache.java</t>
+  </si>
+  <si>
+    <t>OHMap.java</t>
+  </si>
+  <si>
+    <t>PauselessHashMap.java</t>
+  </si>
+  <si>
+    <t>PerfectHashMap.java</t>
+  </si>
+  <si>
+    <t>PersistentHashMap.java</t>
+  </si>
+  <si>
+    <t>PersistentMapException.java</t>
+  </si>
+  <si>
+    <t>PSHOffsetTable.java</t>
+  </si>
+  <si>
+    <t>quadratic_probing (2).py</t>
+  </si>
+  <si>
+    <t>quadratic_probing (3).py</t>
+  </si>
+  <si>
+    <t>quadratic_probing (4).py</t>
+  </si>
+  <si>
+    <t>quadratic_probing.py</t>
+  </si>
+  <si>
+    <t>QuadraticProbing.java</t>
+  </si>
+  <si>
+    <t>RedBlackTree.java</t>
+  </si>
+  <si>
+    <t>RedBlackTreeInteger.java</t>
+  </si>
+  <si>
+    <t>SimpleHashtable (2).java</t>
+  </si>
+  <si>
+    <t>SimpleHashtable.java</t>
+  </si>
+  <si>
+    <t>SortOnValuesInMap.java</t>
+  </si>
+  <si>
+    <t>StoredEmployee.java</t>
+  </si>
+  <si>
+    <t>StringColl.java</t>
+  </si>
+  <si>
+    <t>StringCollClient.java</t>
+  </si>
+  <si>
+    <t>StringSearch.java</t>
+  </si>
+  <si>
+    <t>Student (2).java</t>
+  </si>
+  <si>
+    <t>Student.java</t>
+  </si>
+  <si>
+    <t>Test.java</t>
+  </si>
+  <si>
+    <t>TinyList.java</t>
+  </si>
+  <si>
+    <t>TinyListBuilder.java</t>
+  </si>
+  <si>
+    <t>TinyMap.java</t>
+  </si>
+  <si>
+    <t>TinyMapBuilder.java</t>
+  </si>
+  <si>
+    <t>TinySet.java</t>
+  </si>
+  <si>
+    <t>TinySetBuilder.java</t>
+  </si>
+  <si>
+    <t>TransactionObj.java</t>
+  </si>
+  <si>
+    <t>TreeNode.java</t>
+  </si>
+  <si>
+    <t>UnsortedTableMap.java</t>
+  </si>
+  <si>
+    <t>ValueIterator.java</t>
+  </si>
+  <si>
+    <t>ValueSet.java</t>
+  </si>
+  <si>
+    <t>Vec3I.java</t>
+  </si>
+  <si>
+    <t>View.java</t>
+  </si>
+  <si>
+    <t>WeakConcurrentHashMap.java</t>
+  </si>
+  <si>
+    <t>WeakConcurrentHashMapListener.java</t>
+  </si>
+  <si>
+    <t>WeakConcurrentMap.java</t>
+  </si>
+  <si>
+    <t>WeakConcurrentSet.java</t>
+  </si>
+  <si>
+    <t>WeakHashMapImplementation.java</t>
+  </si>
+  <si>
+    <t>WordCount (2).java</t>
+  </si>
+  <si>
+    <t>WordCount.java</t>
   </si>
 </sst>
 </file>
@@ -745,11 +1099,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E621E51-50FD-4EF4-866F-BB44D85D3FB2}">
-  <dimension ref="A1:O101"/>
+  <dimension ref="A1:O219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J101" sqref="J101"/>
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J220" sqref="J220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4011,6 +4365,3782 @@
         <v>1</v>
       </c>
     </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>113</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>115</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>116</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109">
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110">
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>122</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>123</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>124</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>125</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>127</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>128</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>0</v>
+      </c>
+      <c r="I117">
+        <v>1</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>129</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118">
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>130</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>131</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>133</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>134</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>135</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>0</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>136</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>0</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>137</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>0</v>
+      </c>
+      <c r="I126">
+        <v>0</v>
+      </c>
+      <c r="J126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>138</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <v>0</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>0</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>140</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>0</v>
+      </c>
+      <c r="G129">
+        <v>0</v>
+      </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
+      <c r="I129">
+        <v>0</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>141</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130">
+        <v>0</v>
+      </c>
+      <c r="J130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>142</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
+      <c r="I131">
+        <v>0</v>
+      </c>
+      <c r="J131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>143</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132">
+        <v>0</v>
+      </c>
+      <c r="J132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>144</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133">
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>145</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+      <c r="G134">
+        <v>0</v>
+      </c>
+      <c r="H134">
+        <v>0</v>
+      </c>
+      <c r="I134">
+        <v>1</v>
+      </c>
+      <c r="J134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>146</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+      <c r="I135">
+        <v>1</v>
+      </c>
+      <c r="J135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>147</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+      <c r="G136">
+        <v>0</v>
+      </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>148</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+      <c r="H137">
+        <v>0</v>
+      </c>
+      <c r="I137">
+        <v>0</v>
+      </c>
+      <c r="J137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>149</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138">
+        <v>0</v>
+      </c>
+      <c r="J138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>150</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+      <c r="H139">
+        <v>0</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>151</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>0</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>152</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>153</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>0</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>155</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>156</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>157</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="J146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>158</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>0</v>
+      </c>
+      <c r="I147">
+        <v>0</v>
+      </c>
+      <c r="J147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>159</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>0</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>160</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>161</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <v>0</v>
+      </c>
+      <c r="J150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>162</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>0</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>163</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+      <c r="H152">
+        <v>0</v>
+      </c>
+      <c r="I152">
+        <v>0</v>
+      </c>
+      <c r="J152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>164</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+      <c r="H153">
+        <v>0</v>
+      </c>
+      <c r="I153">
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>165</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154">
+        <v>0</v>
+      </c>
+      <c r="J154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>166</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>0</v>
+      </c>
+      <c r="J155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>167</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156">
+        <v>0</v>
+      </c>
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>168</v>
+      </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+      <c r="H157">
+        <v>0</v>
+      </c>
+      <c r="I157">
+        <v>0</v>
+      </c>
+      <c r="J157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>169</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>0</v>
+      </c>
+      <c r="I158">
+        <v>0</v>
+      </c>
+      <c r="J158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>170</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>0</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>171</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>0</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>0</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>172</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+      <c r="D161">
+        <v>0</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+      <c r="I161">
+        <v>0</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>173</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+      <c r="H162">
+        <v>0</v>
+      </c>
+      <c r="I162">
+        <v>1</v>
+      </c>
+      <c r="J162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>174</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+      <c r="H163">
+        <v>0</v>
+      </c>
+      <c r="I163">
+        <v>0</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>175</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>0</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164">
+        <v>0</v>
+      </c>
+      <c r="I164">
+        <v>0</v>
+      </c>
+      <c r="J164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>176</v>
+      </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+      <c r="I165">
+        <v>0</v>
+      </c>
+      <c r="J165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>177</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>0</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>0</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="H166">
+        <v>0</v>
+      </c>
+      <c r="I166">
+        <v>0</v>
+      </c>
+      <c r="J166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>178</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>0</v>
+      </c>
+      <c r="D167">
+        <v>0</v>
+      </c>
+      <c r="E167">
+        <v>0</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+      <c r="G167">
+        <v>0</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+      <c r="I167">
+        <v>0</v>
+      </c>
+      <c r="J167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>179</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168">
+        <v>0</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="H168">
+        <v>0</v>
+      </c>
+      <c r="I168">
+        <v>0</v>
+      </c>
+      <c r="J168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>180</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>0</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169">
+        <v>0</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+      <c r="G169">
+        <v>0</v>
+      </c>
+      <c r="H169">
+        <v>0</v>
+      </c>
+      <c r="I169">
+        <v>0</v>
+      </c>
+      <c r="J169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>181</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
+      <c r="H170">
+        <v>0</v>
+      </c>
+      <c r="I170">
+        <v>0</v>
+      </c>
+      <c r="J170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>182</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>0</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+      <c r="H171">
+        <v>0</v>
+      </c>
+      <c r="I171">
+        <v>0</v>
+      </c>
+      <c r="J171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>183</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="H172">
+        <v>0</v>
+      </c>
+      <c r="I172">
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>184</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+      <c r="I173">
+        <v>0</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>185</v>
+      </c>
+      <c r="B174">
+        <v>0</v>
+      </c>
+      <c r="C174">
+        <v>0</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+      <c r="G174">
+        <v>0</v>
+      </c>
+      <c r="H174">
+        <v>0</v>
+      </c>
+      <c r="I174">
+        <v>0</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>186</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="C175">
+        <v>0</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+      <c r="G175">
+        <v>0</v>
+      </c>
+      <c r="H175">
+        <v>0</v>
+      </c>
+      <c r="I175">
+        <v>0</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>187</v>
+      </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="G176">
+        <v>0</v>
+      </c>
+      <c r="H176">
+        <v>0</v>
+      </c>
+      <c r="I176">
+        <v>0</v>
+      </c>
+      <c r="J176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>188</v>
+      </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <v>0</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="G177">
+        <v>0</v>
+      </c>
+      <c r="H177">
+        <v>0</v>
+      </c>
+      <c r="I177">
+        <v>0</v>
+      </c>
+      <c r="J177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>189</v>
+      </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+      <c r="H178">
+        <v>0</v>
+      </c>
+      <c r="I178">
+        <v>0</v>
+      </c>
+      <c r="J178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>190</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="G179">
+        <v>0</v>
+      </c>
+      <c r="H179">
+        <v>0</v>
+      </c>
+      <c r="I179">
+        <v>0</v>
+      </c>
+      <c r="J179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>191</v>
+      </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+      <c r="H180">
+        <v>0</v>
+      </c>
+      <c r="I180">
+        <v>0</v>
+      </c>
+      <c r="J180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>192</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181">
+        <v>0</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>193</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
+      <c r="H182">
+        <v>0</v>
+      </c>
+      <c r="I182">
+        <v>0</v>
+      </c>
+      <c r="J182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>194</v>
+      </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>0</v>
+      </c>
+      <c r="J183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>195</v>
+      </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184">
+        <v>0</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
+      </c>
+      <c r="I184">
+        <v>0</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>196</v>
+      </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+      <c r="I185">
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>197</v>
+      </c>
+      <c r="B186">
+        <v>0</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
+      <c r="D186">
+        <v>0</v>
+      </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+      <c r="G186">
+        <v>0</v>
+      </c>
+      <c r="H186">
+        <v>0</v>
+      </c>
+      <c r="I186">
+        <v>0</v>
+      </c>
+      <c r="J186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>198</v>
+      </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>0</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+      <c r="G187">
+        <v>0</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+      <c r="I187">
+        <v>0</v>
+      </c>
+      <c r="J187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>199</v>
+      </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+      <c r="I188">
+        <v>0</v>
+      </c>
+      <c r="J188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>200</v>
+      </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>0</v>
+      </c>
+      <c r="I189">
+        <v>0</v>
+      </c>
+      <c r="J189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>201</v>
+      </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190">
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
+      <c r="H190">
+        <v>0</v>
+      </c>
+      <c r="I190">
+        <v>0</v>
+      </c>
+      <c r="J190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>202</v>
+      </c>
+      <c r="B191">
+        <v>0</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
+      <c r="D191">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>0</v>
+      </c>
+      <c r="I191">
+        <v>0</v>
+      </c>
+      <c r="J191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>203</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>0</v>
+      </c>
+      <c r="I192">
+        <v>0</v>
+      </c>
+      <c r="J192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>204</v>
+      </c>
+      <c r="B193">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>0</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>205</v>
+      </c>
+      <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>0</v>
+      </c>
+      <c r="D194">
+        <v>0</v>
+      </c>
+      <c r="E194">
+        <v>0</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
+      <c r="H194">
+        <v>0</v>
+      </c>
+      <c r="I194">
+        <v>1</v>
+      </c>
+      <c r="J194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>206</v>
+      </c>
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
+      <c r="D195">
+        <v>0</v>
+      </c>
+      <c r="E195">
+        <v>0</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195">
+        <v>0</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="I195">
+        <v>0</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>207</v>
+      </c>
+      <c r="B196">
+        <v>0</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>0</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+      <c r="G196">
+        <v>0</v>
+      </c>
+      <c r="H196">
+        <v>0</v>
+      </c>
+      <c r="I196">
+        <v>0</v>
+      </c>
+      <c r="J196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>208</v>
+      </c>
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+      <c r="G197">
+        <v>0</v>
+      </c>
+      <c r="H197">
+        <v>0</v>
+      </c>
+      <c r="I197">
+        <v>0</v>
+      </c>
+      <c r="J197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>209</v>
+      </c>
+      <c r="B198">
+        <v>0</v>
+      </c>
+      <c r="C198">
+        <v>0</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>0</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>0</v>
+      </c>
+      <c r="I198">
+        <v>0</v>
+      </c>
+      <c r="J198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>210</v>
+      </c>
+      <c r="B199">
+        <v>0</v>
+      </c>
+      <c r="C199">
+        <v>0</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>0</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>0</v>
+      </c>
+      <c r="I199">
+        <v>0</v>
+      </c>
+      <c r="J199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>211</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <v>0</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>0</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+      <c r="G200">
+        <v>0</v>
+      </c>
+      <c r="H200">
+        <v>0</v>
+      </c>
+      <c r="I200">
+        <v>0</v>
+      </c>
+      <c r="J200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>212</v>
+      </c>
+      <c r="B201">
+        <v>0</v>
+      </c>
+      <c r="C201">
+        <v>0</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201">
+        <v>0</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+      <c r="G201">
+        <v>0</v>
+      </c>
+      <c r="H201">
+        <v>0</v>
+      </c>
+      <c r="I201">
+        <v>0</v>
+      </c>
+      <c r="J201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>213</v>
+      </c>
+      <c r="B202">
+        <v>0</v>
+      </c>
+      <c r="C202">
+        <v>0</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202">
+        <v>0</v>
+      </c>
+      <c r="F202">
+        <v>0</v>
+      </c>
+      <c r="G202">
+        <v>0</v>
+      </c>
+      <c r="H202">
+        <v>0</v>
+      </c>
+      <c r="I202">
+        <v>0</v>
+      </c>
+      <c r="J202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>214</v>
+      </c>
+      <c r="B203">
+        <v>0</v>
+      </c>
+      <c r="C203">
+        <v>0</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203">
+        <v>0</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <v>0</v>
+      </c>
+      <c r="I203">
+        <v>0</v>
+      </c>
+      <c r="J203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>215</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204">
+        <v>0</v>
+      </c>
+      <c r="F204">
+        <v>0</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>0</v>
+      </c>
+      <c r="I204">
+        <v>0</v>
+      </c>
+      <c r="J204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>216</v>
+      </c>
+      <c r="B205">
+        <v>0</v>
+      </c>
+      <c r="C205">
+        <v>0</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205">
+        <v>0</v>
+      </c>
+      <c r="F205">
+        <v>0</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
+      <c r="H205">
+        <v>0</v>
+      </c>
+      <c r="I205">
+        <v>0</v>
+      </c>
+      <c r="J205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>217</v>
+      </c>
+      <c r="B206">
+        <v>0</v>
+      </c>
+      <c r="C206">
+        <v>0</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>0</v>
+      </c>
+      <c r="F206">
+        <v>0</v>
+      </c>
+      <c r="G206">
+        <v>0</v>
+      </c>
+      <c r="H206">
+        <v>0</v>
+      </c>
+      <c r="I206">
+        <v>0</v>
+      </c>
+      <c r="J206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>218</v>
+      </c>
+      <c r="B207">
+        <v>0</v>
+      </c>
+      <c r="C207">
+        <v>0</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207">
+        <v>0</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+      <c r="G207">
+        <v>0</v>
+      </c>
+      <c r="H207">
+        <v>0</v>
+      </c>
+      <c r="I207">
+        <v>0</v>
+      </c>
+      <c r="J207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>219</v>
+      </c>
+      <c r="B208">
+        <v>0</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="E208">
+        <v>0</v>
+      </c>
+      <c r="F208">
+        <v>0</v>
+      </c>
+      <c r="G208">
+        <v>0</v>
+      </c>
+      <c r="H208">
+        <v>0</v>
+      </c>
+      <c r="I208">
+        <v>0</v>
+      </c>
+      <c r="J208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>220</v>
+      </c>
+      <c r="B209">
+        <v>0</v>
+      </c>
+      <c r="C209">
+        <v>0</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <v>0</v>
+      </c>
+      <c r="G209">
+        <v>0</v>
+      </c>
+      <c r="H209">
+        <v>0</v>
+      </c>
+      <c r="I209">
+        <v>0</v>
+      </c>
+      <c r="J209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>221</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>0</v>
+      </c>
+      <c r="F210">
+        <v>0</v>
+      </c>
+      <c r="G210">
+        <v>0</v>
+      </c>
+      <c r="H210">
+        <v>0</v>
+      </c>
+      <c r="I210">
+        <v>0</v>
+      </c>
+      <c r="J210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>222</v>
+      </c>
+      <c r="B211">
+        <v>0</v>
+      </c>
+      <c r="C211">
+        <v>0</v>
+      </c>
+      <c r="D211">
+        <v>0</v>
+      </c>
+      <c r="E211">
+        <v>0</v>
+      </c>
+      <c r="F211">
+        <v>0</v>
+      </c>
+      <c r="G211">
+        <v>0</v>
+      </c>
+      <c r="H211">
+        <v>0</v>
+      </c>
+      <c r="I211">
+        <v>0</v>
+      </c>
+      <c r="J211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>223</v>
+      </c>
+      <c r="B212">
+        <v>0</v>
+      </c>
+      <c r="C212">
+        <v>0</v>
+      </c>
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="E212">
+        <v>0</v>
+      </c>
+      <c r="F212">
+        <v>0</v>
+      </c>
+      <c r="G212">
+        <v>0</v>
+      </c>
+      <c r="H212">
+        <v>0</v>
+      </c>
+      <c r="I212">
+        <v>0</v>
+      </c>
+      <c r="J212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>224</v>
+      </c>
+      <c r="B213">
+        <v>0</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>0</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="G213">
+        <v>0</v>
+      </c>
+      <c r="H213">
+        <v>0</v>
+      </c>
+      <c r="I213">
+        <v>0</v>
+      </c>
+      <c r="J213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>225</v>
+      </c>
+      <c r="B214">
+        <v>0</v>
+      </c>
+      <c r="C214">
+        <v>0</v>
+      </c>
+      <c r="D214">
+        <v>0</v>
+      </c>
+      <c r="E214">
+        <v>0</v>
+      </c>
+      <c r="F214">
+        <v>0</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
+      <c r="H214">
+        <v>0</v>
+      </c>
+      <c r="I214">
+        <v>0</v>
+      </c>
+      <c r="J214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>226</v>
+      </c>
+      <c r="B215">
+        <v>0</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="E215">
+        <v>0</v>
+      </c>
+      <c r="F215">
+        <v>0</v>
+      </c>
+      <c r="G215">
+        <v>0</v>
+      </c>
+      <c r="H215">
+        <v>0</v>
+      </c>
+      <c r="I215">
+        <v>0</v>
+      </c>
+      <c r="J215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>227</v>
+      </c>
+      <c r="B216">
+        <v>0</v>
+      </c>
+      <c r="C216">
+        <v>0</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>0</v>
+      </c>
+      <c r="F216">
+        <v>0</v>
+      </c>
+      <c r="G216">
+        <v>0</v>
+      </c>
+      <c r="H216">
+        <v>0</v>
+      </c>
+      <c r="I216">
+        <v>0</v>
+      </c>
+      <c r="J216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>228</v>
+      </c>
+      <c r="B217">
+        <v>0</v>
+      </c>
+      <c r="C217">
+        <v>0</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>0</v>
+      </c>
+      <c r="F217">
+        <v>0</v>
+      </c>
+      <c r="G217">
+        <v>0</v>
+      </c>
+      <c r="H217">
+        <v>0</v>
+      </c>
+      <c r="I217">
+        <v>0</v>
+      </c>
+      <c r="J217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>229</v>
+      </c>
+      <c r="B218">
+        <v>0</v>
+      </c>
+      <c r="C218">
+        <v>0</v>
+      </c>
+      <c r="D218">
+        <v>0</v>
+      </c>
+      <c r="E218">
+        <v>0</v>
+      </c>
+      <c r="F218">
+        <v>0</v>
+      </c>
+      <c r="G218">
+        <v>0</v>
+      </c>
+      <c r="H218">
+        <v>0</v>
+      </c>
+      <c r="I218">
+        <v>0</v>
+      </c>
+      <c r="J218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>230</v>
+      </c>
+      <c r="B219">
+        <v>0</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>0</v>
+      </c>
+      <c r="F219">
+        <v>0</v>
+      </c>
+      <c r="G219">
+        <v>0</v>
+      </c>
+      <c r="H219">
+        <v>0</v>
+      </c>
+      <c r="I219">
+        <v>0</v>
+      </c>
+      <c r="J219">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted (1) label re: C# language; Added 82 labeled data; Total 300
</commit_message>
<xml_diff>
--- a/John.xlsx
+++ b/John.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d03dc4ea78fd367a/Documents/S. Y. 2021-2022/1st Sem/Senior Thesis/data labeling/Final data labeling/data-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="534" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E371093B-E5D6-4A54-B7A5-1AAF51972A38}"/>
+  <xr:revisionPtr revIDLastSave="736" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2012E89B-0EA3-4E8F-AA8F-9008CC1318C9}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="3705" windowWidth="21600" windowHeight="11385" xr2:uid="{77CB7C1E-B4AD-45B5-9992-3E1454331525}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="308">
   <si>
     <t>Filename</t>
   </si>
@@ -213,9 +213,6 @@
     <t>DetachedThreadLocal.java</t>
   </si>
   <si>
-    <t>Dict.cs</t>
-  </si>
-  <si>
     <t>dictionary.py</t>
   </si>
   <si>
@@ -727,6 +724,240 @@
   </si>
   <si>
     <t>WordCount.java</t>
+  </si>
+  <si>
+    <t>ArrayList.java</t>
+  </si>
+  <si>
+    <t>base_linked_list.py</t>
+  </si>
+  <si>
+    <t>CircleLinkedList (2).java</t>
+  </si>
+  <si>
+    <t>CircleLinkedList (3).java</t>
+  </si>
+  <si>
+    <t>CircleLinkedList (4).java</t>
+  </si>
+  <si>
+    <t>CircleLinkedList (5).java</t>
+  </si>
+  <si>
+    <t>CircleLinkedList.java</t>
+  </si>
+  <si>
+    <t>circular_linked_list.py</t>
+  </si>
+  <si>
+    <t>CircularDoublyLinkedList.java</t>
+  </si>
+  <si>
+    <t>CircularLinkedList (2).java</t>
+  </si>
+  <si>
+    <t>CircularLinkedList (3).java</t>
+  </si>
+  <si>
+    <t>CircularLinkedList (4).java</t>
+  </si>
+  <si>
+    <t>CircularLinkedList.java</t>
+  </si>
+  <si>
+    <t>CircularSinglyLinkedList.java</t>
+  </si>
+  <si>
+    <t>CoinFlipper.java</t>
+  </si>
+  <si>
+    <t>CursorLinkedList.java</t>
+  </si>
+  <si>
+    <t>DLinkedList.java</t>
+  </si>
+  <si>
+    <t>DLinkedListTest.java</t>
+  </si>
+  <si>
+    <t>doubly_linked_list (2).py</t>
+  </si>
+  <si>
+    <t>doubly_linked_list (3).py</t>
+  </si>
+  <si>
+    <t>doubly_linked_list (4).py</t>
+  </si>
+  <si>
+    <t>doubly_linked_list.py</t>
+  </si>
+  <si>
+    <t>doubly_linked.py</t>
+  </si>
+  <si>
+    <t>doubly-linked-list.js</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (2).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (2).js</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (3).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (4).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (5).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (6).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (7).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (8).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (9).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (10).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (11).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList (12).java</t>
+  </si>
+  <si>
+    <t>DoublyLinkedList.js</t>
+  </si>
+  <si>
+    <t>DoublyLinkedListImplementation.java</t>
+  </si>
+  <si>
+    <t>Employee (2).java</t>
+  </si>
+  <si>
+    <t>Employee (3).java</t>
+  </si>
+  <si>
+    <t>Employee (4).java</t>
+  </si>
+  <si>
+    <t>Employee.java</t>
+  </si>
+  <si>
+    <t>EmployeeDoublyLinkedList (2).java</t>
+  </si>
+  <si>
+    <t>EmployeeDoublyLinkedList (3).java</t>
+  </si>
+  <si>
+    <t>EmployeeDoublyLinkedList.java</t>
+  </si>
+  <si>
+    <t>EmployeeLinkedList (2).java</t>
+  </si>
+  <si>
+    <t>EmployeeLinkedList.java</t>
+  </si>
+  <si>
+    <t>EmployeeNode (2).java</t>
+  </si>
+  <si>
+    <t>EmployeeNode (3).java</t>
+  </si>
+  <si>
+    <t>EmployeeNode (4).java</t>
+  </si>
+  <si>
+    <t>EmployeeNode.java</t>
+  </si>
+  <si>
+    <t>EmptyListException.java</t>
+  </si>
+  <si>
+    <t>Intcoll4.java</t>
+  </si>
+  <si>
+    <t>Intcoll5.java</t>
+  </si>
+  <si>
+    <t>IntegerLinkedList.java</t>
+  </si>
+  <si>
+    <t>IntegerNode.java</t>
+  </si>
+  <si>
+    <t>is_Palindrome (2).py</t>
+  </si>
+  <si>
+    <t>is_Palindrome (3).py</t>
+  </si>
+  <si>
+    <t>is_Palindrome.py</t>
+  </si>
+  <si>
+    <t>linked_list (2).py</t>
+  </si>
+  <si>
+    <t>linked_list (3).py</t>
+  </si>
+  <si>
+    <t>linked_list (4).py</t>
+  </si>
+  <si>
+    <t>linked_list (5).py</t>
+  </si>
+  <si>
+    <t>linked_list_reverse.py</t>
+  </si>
+  <si>
+    <t>linked_list.py</t>
+  </si>
+  <si>
+    <t>linked-list.js</t>
+  </si>
+  <si>
+    <t>LinkedList (2).js</t>
+  </si>
+  <si>
+    <t>linkedList (3).js</t>
+  </si>
+  <si>
+    <t>LinkedList (5).java</t>
+  </si>
+  <si>
+    <t>LinkedList (6).java</t>
+  </si>
+  <si>
+    <t>linkedlist (7).java</t>
+  </si>
+  <si>
+    <t>linkedList.js</t>
+  </si>
+  <si>
+    <t>linkedlist.py</t>
+  </si>
+  <si>
+    <t>LinkedListImplementation.java</t>
+  </si>
+  <si>
+    <t>LinkedListInterface (2).java</t>
+  </si>
+  <si>
+    <t>LinkedListInterface.java</t>
+  </si>
+  <si>
+    <t>LinkedListNode.java</t>
+  </si>
+  <si>
+    <t>linklistbag.py</t>
   </si>
 </sst>
 </file>
@@ -1099,11 +1330,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E621E51-50FD-4EF4-866F-BB44D85D3FB2}">
-  <dimension ref="A1:O219"/>
+  <dimension ref="A1:O301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J220" sqref="J220"/>
+      <pane ySplit="1" topLeftCell="A286" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I301" sqref="I301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="J49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2826,7 +3057,7 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2986,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -3018,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="J59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3114,7 +3345,7 @@
         <v>0</v>
       </c>
       <c r="J62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -3146,7 +3377,7 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -3242,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="J66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -3274,7 +3505,7 @@
         <v>0</v>
       </c>
       <c r="J67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -3626,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="J78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -3658,7 +3889,7 @@
         <v>0</v>
       </c>
       <c r="J79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -3754,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="J82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -3850,7 +4081,7 @@
         <v>0</v>
       </c>
       <c r="J85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -3882,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="J86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -3914,7 +4145,7 @@
         <v>0</v>
       </c>
       <c r="J87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -4042,7 +4273,7 @@
         <v>0</v>
       </c>
       <c r="J91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
@@ -4074,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="J92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -4202,7 +4433,7 @@
         <v>0</v>
       </c>
       <c r="J96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -4266,7 +4497,7 @@
         <v>0</v>
       </c>
       <c r="J98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -4426,7 +4657,7 @@
         <v>0</v>
       </c>
       <c r="J103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
@@ -4522,7 +4753,7 @@
         <v>0</v>
       </c>
       <c r="J106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
@@ -4586,7 +4817,7 @@
         <v>0</v>
       </c>
       <c r="J108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
@@ -4682,7 +4913,7 @@
         <v>0</v>
       </c>
       <c r="J111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -4839,10 +5070,10 @@
         <v>0</v>
       </c>
       <c r="I116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
@@ -4871,7 +5102,7 @@
         <v>0</v>
       </c>
       <c r="I117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J117">
         <v>0</v>
@@ -4970,7 +5201,7 @@
         <v>0</v>
       </c>
       <c r="J120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
@@ -5002,7 +5233,7 @@
         <v>0</v>
       </c>
       <c r="J121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
@@ -5034,7 +5265,7 @@
         <v>0</v>
       </c>
       <c r="J122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -5098,7 +5329,7 @@
         <v>0</v>
       </c>
       <c r="J124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -5162,7 +5393,7 @@
         <v>0</v>
       </c>
       <c r="J126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
@@ -5194,7 +5425,7 @@
         <v>0</v>
       </c>
       <c r="J127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
@@ -5258,7 +5489,7 @@
         <v>0</v>
       </c>
       <c r="J129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
@@ -5290,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="J130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
@@ -5322,7 +5553,7 @@
         <v>0</v>
       </c>
       <c r="J131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
@@ -5351,10 +5582,10 @@
         <v>0</v>
       </c>
       <c r="I132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J132">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
@@ -5479,7 +5710,7 @@
         <v>0</v>
       </c>
       <c r="I136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J136">
         <v>0</v>
@@ -5514,7 +5745,7 @@
         <v>0</v>
       </c>
       <c r="J137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
@@ -5578,7 +5809,7 @@
         <v>0</v>
       </c>
       <c r="J139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
@@ -5610,7 +5841,7 @@
         <v>0</v>
       </c>
       <c r="J140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
@@ -5642,7 +5873,7 @@
         <v>0</v>
       </c>
       <c r="J141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
@@ -5706,7 +5937,7 @@
         <v>0</v>
       </c>
       <c r="J143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
@@ -5834,7 +6065,7 @@
         <v>0</v>
       </c>
       <c r="J147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
@@ -5866,7 +6097,7 @@
         <v>0</v>
       </c>
       <c r="J148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
@@ -5962,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="J151">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
@@ -6026,7 +6257,7 @@
         <v>0</v>
       </c>
       <c r="J153">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
@@ -6162,7 +6393,7 @@
         <v>169</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -6186,7 +6417,7 @@
         <v>0</v>
       </c>
       <c r="J158">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
@@ -6194,7 +6425,7 @@
         <v>170</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -6279,7 +6510,7 @@
         <v>0</v>
       </c>
       <c r="I161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J161">
         <v>0</v>
@@ -6311,7 +6542,7 @@
         <v>0</v>
       </c>
       <c r="I162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J162">
         <v>0</v>
@@ -6346,7 +6577,7 @@
         <v>0</v>
       </c>
       <c r="J163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
@@ -6378,7 +6609,7 @@
         <v>0</v>
       </c>
       <c r="J164">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
@@ -6442,7 +6673,7 @@
         <v>0</v>
       </c>
       <c r="J166">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
@@ -6538,7 +6769,7 @@
         <v>0</v>
       </c>
       <c r="J169">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
@@ -6762,7 +6993,7 @@
         <v>0</v>
       </c>
       <c r="J176">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
@@ -6890,7 +7121,7 @@
         <v>0</v>
       </c>
       <c r="J180">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
@@ -6898,7 +7129,7 @@
         <v>192</v>
       </c>
       <c r="B181">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C181">
         <v>0</v>
@@ -6922,7 +7153,7 @@
         <v>0</v>
       </c>
       <c r="J181">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
@@ -6930,7 +7161,7 @@
         <v>193</v>
       </c>
       <c r="B182">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C182">
         <v>0</v>
@@ -6954,7 +7185,7 @@
         <v>0</v>
       </c>
       <c r="J182">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
@@ -7114,7 +7345,7 @@
         <v>0</v>
       </c>
       <c r="J187">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
@@ -7210,7 +7441,7 @@
         <v>0</v>
       </c>
       <c r="J190">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
@@ -7242,7 +7473,7 @@
         <v>0</v>
       </c>
       <c r="J191">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
@@ -7274,7 +7505,7 @@
         <v>0</v>
       </c>
       <c r="J192">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
@@ -7303,7 +7534,7 @@
         <v>0</v>
       </c>
       <c r="I193">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J193">
         <v>0</v>
@@ -7335,7 +7566,7 @@
         <v>0</v>
       </c>
       <c r="I194">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J194">
         <v>0</v>
@@ -7562,7 +7793,7 @@
         <v>0</v>
       </c>
       <c r="J201">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
@@ -7722,7 +7953,7 @@
         <v>0</v>
       </c>
       <c r="J206">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
@@ -7754,7 +7985,7 @@
         <v>0</v>
       </c>
       <c r="J207">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
@@ -7850,7 +8081,7 @@
         <v>0</v>
       </c>
       <c r="J210">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
@@ -7914,7 +8145,7 @@
         <v>0</v>
       </c>
       <c r="J212">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
@@ -7946,7 +8177,7 @@
         <v>0</v>
       </c>
       <c r="J213">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
@@ -7978,7 +8209,7 @@
         <v>0</v>
       </c>
       <c r="J214">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
@@ -8010,7 +8241,7 @@
         <v>0</v>
       </c>
       <c r="J215">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
@@ -8042,7 +8273,7 @@
         <v>0</v>
       </c>
       <c r="J216">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
@@ -8074,7 +8305,7 @@
         <v>0</v>
       </c>
       <c r="J217">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
@@ -8106,7 +8337,7 @@
         <v>0</v>
       </c>
       <c r="J218">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
@@ -8138,7 +8369,2631 @@
         <v>0</v>
       </c>
       <c r="J219">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>231</v>
+      </c>
+      <c r="B220">
+        <v>0</v>
+      </c>
+      <c r="C220">
+        <v>0</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>0</v>
+      </c>
+      <c r="F220">
+        <v>0</v>
+      </c>
+      <c r="G220">
+        <v>0</v>
+      </c>
+      <c r="H220">
+        <v>0</v>
+      </c>
+      <c r="I220">
+        <v>1</v>
+      </c>
+      <c r="J220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>232</v>
+      </c>
+      <c r="B221">
+        <v>0</v>
+      </c>
+      <c r="C221">
+        <v>0</v>
+      </c>
+      <c r="D221">
+        <v>0</v>
+      </c>
+      <c r="E221">
+        <v>0</v>
+      </c>
+      <c r="F221">
+        <v>0</v>
+      </c>
+      <c r="G221">
+        <v>0</v>
+      </c>
+      <c r="H221">
+        <v>0</v>
+      </c>
+      <c r="I221">
+        <v>1</v>
+      </c>
+      <c r="J221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>233</v>
+      </c>
+      <c r="B222">
+        <v>0</v>
+      </c>
+      <c r="C222">
+        <v>0</v>
+      </c>
+      <c r="D222">
+        <v>0</v>
+      </c>
+      <c r="E222">
+        <v>0</v>
+      </c>
+      <c r="F222">
+        <v>0</v>
+      </c>
+      <c r="G222">
+        <v>0</v>
+      </c>
+      <c r="H222">
+        <v>0</v>
+      </c>
+      <c r="I222">
+        <v>1</v>
+      </c>
+      <c r="J222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>234</v>
+      </c>
+      <c r="B223">
+        <v>0</v>
+      </c>
+      <c r="C223">
+        <v>0</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>0</v>
+      </c>
+      <c r="F223">
+        <v>0</v>
+      </c>
+      <c r="G223">
+        <v>0</v>
+      </c>
+      <c r="H223">
+        <v>0</v>
+      </c>
+      <c r="I223">
+        <v>1</v>
+      </c>
+      <c r="J223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>235</v>
+      </c>
+      <c r="B224">
+        <v>0</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>0</v>
+      </c>
+      <c r="F224">
+        <v>0</v>
+      </c>
+      <c r="G224">
+        <v>0</v>
+      </c>
+      <c r="H224">
+        <v>0</v>
+      </c>
+      <c r="I224">
+        <v>1</v>
+      </c>
+      <c r="J224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>236</v>
+      </c>
+      <c r="B225">
+        <v>0</v>
+      </c>
+      <c r="C225">
+        <v>0</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
+      <c r="E225">
+        <v>0</v>
+      </c>
+      <c r="F225">
+        <v>0</v>
+      </c>
+      <c r="G225">
+        <v>0</v>
+      </c>
+      <c r="H225">
+        <v>0</v>
+      </c>
+      <c r="I225">
+        <v>1</v>
+      </c>
+      <c r="J225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>237</v>
+      </c>
+      <c r="B226">
+        <v>0</v>
+      </c>
+      <c r="C226">
+        <v>0</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
+      <c r="E226">
+        <v>0</v>
+      </c>
+      <c r="F226">
+        <v>0</v>
+      </c>
+      <c r="G226">
+        <v>0</v>
+      </c>
+      <c r="H226">
+        <v>0</v>
+      </c>
+      <c r="I226">
+        <v>1</v>
+      </c>
+      <c r="J226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>238</v>
+      </c>
+      <c r="B227">
+        <v>0</v>
+      </c>
+      <c r="C227">
+        <v>0</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+      <c r="E227">
+        <v>0</v>
+      </c>
+      <c r="F227">
+        <v>0</v>
+      </c>
+      <c r="G227">
+        <v>0</v>
+      </c>
+      <c r="H227">
+        <v>0</v>
+      </c>
+      <c r="I227">
+        <v>1</v>
+      </c>
+      <c r="J227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>239</v>
+      </c>
+      <c r="B228">
+        <v>0</v>
+      </c>
+      <c r="C228">
+        <v>0</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
+      <c r="E228">
+        <v>0</v>
+      </c>
+      <c r="F228">
+        <v>0</v>
+      </c>
+      <c r="G228">
+        <v>0</v>
+      </c>
+      <c r="H228">
+        <v>0</v>
+      </c>
+      <c r="I228">
+        <v>1</v>
+      </c>
+      <c r="J228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>240</v>
+      </c>
+      <c r="B229">
+        <v>0</v>
+      </c>
+      <c r="C229">
+        <v>0</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>0</v>
+      </c>
+      <c r="F229">
+        <v>0</v>
+      </c>
+      <c r="G229">
+        <v>1</v>
+      </c>
+      <c r="H229">
+        <v>0</v>
+      </c>
+      <c r="I229">
+        <v>1</v>
+      </c>
+      <c r="J229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>241</v>
+      </c>
+      <c r="B230">
+        <v>0</v>
+      </c>
+      <c r="C230">
+        <v>0</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>0</v>
+      </c>
+      <c r="F230">
+        <v>0</v>
+      </c>
+      <c r="G230">
+        <v>0</v>
+      </c>
+      <c r="H230">
+        <v>0</v>
+      </c>
+      <c r="I230">
+        <v>1</v>
+      </c>
+      <c r="J230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>242</v>
+      </c>
+      <c r="B231">
+        <v>0</v>
+      </c>
+      <c r="C231">
+        <v>0</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="E231">
+        <v>0</v>
+      </c>
+      <c r="F231">
+        <v>0</v>
+      </c>
+      <c r="G231">
+        <v>0</v>
+      </c>
+      <c r="H231">
+        <v>0</v>
+      </c>
+      <c r="I231">
+        <v>1</v>
+      </c>
+      <c r="J231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>243</v>
+      </c>
+      <c r="B232">
+        <v>0</v>
+      </c>
+      <c r="C232">
+        <v>0</v>
+      </c>
+      <c r="D232">
+        <v>0</v>
+      </c>
+      <c r="E232">
+        <v>0</v>
+      </c>
+      <c r="F232">
+        <v>0</v>
+      </c>
+      <c r="G232">
+        <v>0</v>
+      </c>
+      <c r="H232">
+        <v>0</v>
+      </c>
+      <c r="I232">
+        <v>1</v>
+      </c>
+      <c r="J232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>244</v>
+      </c>
+      <c r="B233">
+        <v>0</v>
+      </c>
+      <c r="C233">
+        <v>0</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>0</v>
+      </c>
+      <c r="F233">
+        <v>0</v>
+      </c>
+      <c r="G233">
+        <v>0</v>
+      </c>
+      <c r="H233">
+        <v>0</v>
+      </c>
+      <c r="I233">
+        <v>0</v>
+      </c>
+      <c r="J233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>245</v>
+      </c>
+      <c r="B234">
+        <v>0</v>
+      </c>
+      <c r="C234">
+        <v>0</v>
+      </c>
+      <c r="D234">
+        <v>0</v>
+      </c>
+      <c r="E234">
+        <v>0</v>
+      </c>
+      <c r="F234">
+        <v>0</v>
+      </c>
+      <c r="G234">
+        <v>0</v>
+      </c>
+      <c r="H234">
+        <v>0</v>
+      </c>
+      <c r="I234">
+        <v>1</v>
+      </c>
+      <c r="J234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>246</v>
+      </c>
+      <c r="B235">
+        <v>0</v>
+      </c>
+      <c r="C235">
+        <v>0</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>0</v>
+      </c>
+      <c r="F235">
+        <v>0</v>
+      </c>
+      <c r="G235">
+        <v>1</v>
+      </c>
+      <c r="H235">
+        <v>0</v>
+      </c>
+      <c r="I235">
+        <v>1</v>
+      </c>
+      <c r="J235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>247</v>
+      </c>
+      <c r="B236">
+        <v>0</v>
+      </c>
+      <c r="C236">
+        <v>0</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>0</v>
+      </c>
+      <c r="F236">
+        <v>0</v>
+      </c>
+      <c r="G236">
+        <v>0</v>
+      </c>
+      <c r="H236">
+        <v>0</v>
+      </c>
+      <c r="I236">
+        <v>0</v>
+      </c>
+      <c r="J236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>248</v>
+      </c>
+      <c r="B237">
+        <v>0</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+      <c r="E237">
+        <v>0</v>
+      </c>
+      <c r="F237">
+        <v>0</v>
+      </c>
+      <c r="G237">
+        <v>0</v>
+      </c>
+      <c r="H237">
+        <v>0</v>
+      </c>
+      <c r="I237">
+        <v>1</v>
+      </c>
+      <c r="J237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>249</v>
+      </c>
+      <c r="B238">
+        <v>0</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>0</v>
+      </c>
+      <c r="F238">
+        <v>0</v>
+      </c>
+      <c r="G238">
+        <v>0</v>
+      </c>
+      <c r="H238">
+        <v>0</v>
+      </c>
+      <c r="I238">
+        <v>1</v>
+      </c>
+      <c r="J238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>250</v>
+      </c>
+      <c r="B239">
+        <v>0</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>0</v>
+      </c>
+      <c r="F239">
+        <v>0</v>
+      </c>
+      <c r="G239">
+        <v>0</v>
+      </c>
+      <c r="H239">
+        <v>0</v>
+      </c>
+      <c r="I239">
+        <v>1</v>
+      </c>
+      <c r="J239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>251</v>
+      </c>
+      <c r="B240">
+        <v>0</v>
+      </c>
+      <c r="C240">
+        <v>0</v>
+      </c>
+      <c r="D240">
+        <v>0</v>
+      </c>
+      <c r="E240">
+        <v>0</v>
+      </c>
+      <c r="F240">
+        <v>0</v>
+      </c>
+      <c r="G240">
+        <v>0</v>
+      </c>
+      <c r="H240">
+        <v>0</v>
+      </c>
+      <c r="I240">
+        <v>1</v>
+      </c>
+      <c r="J240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>252</v>
+      </c>
+      <c r="B241">
+        <v>0</v>
+      </c>
+      <c r="C241">
+        <v>0</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+      <c r="E241">
+        <v>0</v>
+      </c>
+      <c r="F241">
+        <v>0</v>
+      </c>
+      <c r="G241">
+        <v>1</v>
+      </c>
+      <c r="H241">
+        <v>0</v>
+      </c>
+      <c r="I241">
+        <v>1</v>
+      </c>
+      <c r="J241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>253</v>
+      </c>
+      <c r="B242">
+        <v>0</v>
+      </c>
+      <c r="C242">
+        <v>0</v>
+      </c>
+      <c r="D242">
+        <v>0</v>
+      </c>
+      <c r="E242">
+        <v>0</v>
+      </c>
+      <c r="F242">
+        <v>0</v>
+      </c>
+      <c r="G242">
+        <v>0</v>
+      </c>
+      <c r="H242">
+        <v>0</v>
+      </c>
+      <c r="I242">
+        <v>1</v>
+      </c>
+      <c r="J242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>254</v>
+      </c>
+      <c r="B243">
+        <v>0</v>
+      </c>
+      <c r="C243">
+        <v>0</v>
+      </c>
+      <c r="D243">
+        <v>0</v>
+      </c>
+      <c r="E243">
+        <v>0</v>
+      </c>
+      <c r="F243">
+        <v>0</v>
+      </c>
+      <c r="G243">
+        <v>0</v>
+      </c>
+      <c r="H243">
+        <v>0</v>
+      </c>
+      <c r="I243">
+        <v>1</v>
+      </c>
+      <c r="J243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>255</v>
+      </c>
+      <c r="B244">
+        <v>0</v>
+      </c>
+      <c r="C244">
+        <v>0</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+      <c r="E244">
+        <v>0</v>
+      </c>
+      <c r="F244">
+        <v>0</v>
+      </c>
+      <c r="G244">
+        <v>0</v>
+      </c>
+      <c r="H244">
+        <v>0</v>
+      </c>
+      <c r="I244">
+        <v>1</v>
+      </c>
+      <c r="J244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>256</v>
+      </c>
+      <c r="B245">
+        <v>0</v>
+      </c>
+      <c r="C245">
+        <v>0</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>0</v>
+      </c>
+      <c r="F245">
+        <v>0</v>
+      </c>
+      <c r="G245">
+        <v>0</v>
+      </c>
+      <c r="H245">
+        <v>0</v>
+      </c>
+      <c r="I245">
+        <v>1</v>
+      </c>
+      <c r="J245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>257</v>
+      </c>
+      <c r="B246">
+        <v>0</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+      <c r="D246">
+        <v>0</v>
+      </c>
+      <c r="E246">
+        <v>0</v>
+      </c>
+      <c r="F246">
+        <v>0</v>
+      </c>
+      <c r="G246">
+        <v>0</v>
+      </c>
+      <c r="H246">
+        <v>0</v>
+      </c>
+      <c r="I246">
+        <v>1</v>
+      </c>
+      <c r="J246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>258</v>
+      </c>
+      <c r="B247">
+        <v>0</v>
+      </c>
+      <c r="C247">
+        <v>0</v>
+      </c>
+      <c r="D247">
+        <v>0</v>
+      </c>
+      <c r="E247">
+        <v>0</v>
+      </c>
+      <c r="F247">
+        <v>0</v>
+      </c>
+      <c r="G247">
+        <v>0</v>
+      </c>
+      <c r="H247">
+        <v>0</v>
+      </c>
+      <c r="I247">
+        <v>1</v>
+      </c>
+      <c r="J247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>259</v>
+      </c>
+      <c r="B248">
+        <v>0</v>
+      </c>
+      <c r="C248">
+        <v>0</v>
+      </c>
+      <c r="D248">
+        <v>0</v>
+      </c>
+      <c r="E248">
+        <v>0</v>
+      </c>
+      <c r="F248">
+        <v>0</v>
+      </c>
+      <c r="G248">
+        <v>0</v>
+      </c>
+      <c r="H248">
+        <v>0</v>
+      </c>
+      <c r="I248">
+        <v>1</v>
+      </c>
+      <c r="J248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>260</v>
+      </c>
+      <c r="B249">
+        <v>0</v>
+      </c>
+      <c r="C249">
+        <v>0</v>
+      </c>
+      <c r="D249">
+        <v>0</v>
+      </c>
+      <c r="E249">
+        <v>0</v>
+      </c>
+      <c r="F249">
+        <v>0</v>
+      </c>
+      <c r="G249">
+        <v>1</v>
+      </c>
+      <c r="H249">
+        <v>0</v>
+      </c>
+      <c r="I249">
+        <v>1</v>
+      </c>
+      <c r="J249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>261</v>
+      </c>
+      <c r="B250">
+        <v>0</v>
+      </c>
+      <c r="C250">
+        <v>0</v>
+      </c>
+      <c r="D250">
+        <v>0</v>
+      </c>
+      <c r="E250">
+        <v>0</v>
+      </c>
+      <c r="F250">
+        <v>0</v>
+      </c>
+      <c r="G250">
+        <v>0</v>
+      </c>
+      <c r="H250">
+        <v>0</v>
+      </c>
+      <c r="I250">
+        <v>0</v>
+      </c>
+      <c r="J250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>262</v>
+      </c>
+      <c r="B251">
+        <v>0</v>
+      </c>
+      <c r="C251">
+        <v>0</v>
+      </c>
+      <c r="D251">
+        <v>0</v>
+      </c>
+      <c r="E251">
+        <v>0</v>
+      </c>
+      <c r="F251">
+        <v>0</v>
+      </c>
+      <c r="G251">
+        <v>0</v>
+      </c>
+      <c r="H251">
+        <v>0</v>
+      </c>
+      <c r="I251">
+        <v>1</v>
+      </c>
+      <c r="J251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>263</v>
+      </c>
+      <c r="B252">
+        <v>0</v>
+      </c>
+      <c r="C252">
+        <v>0</v>
+      </c>
+      <c r="D252">
+        <v>0</v>
+      </c>
+      <c r="E252">
+        <v>0</v>
+      </c>
+      <c r="F252">
+        <v>0</v>
+      </c>
+      <c r="G252">
+        <v>1</v>
+      </c>
+      <c r="H252">
+        <v>0</v>
+      </c>
+      <c r="I252">
+        <v>1</v>
+      </c>
+      <c r="J252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>264</v>
+      </c>
+      <c r="B253">
+        <v>0</v>
+      </c>
+      <c r="C253">
+        <v>0</v>
+      </c>
+      <c r="D253">
+        <v>0</v>
+      </c>
+      <c r="E253">
+        <v>0</v>
+      </c>
+      <c r="F253">
+        <v>0</v>
+      </c>
+      <c r="G253">
+        <v>1</v>
+      </c>
+      <c r="H253">
+        <v>0</v>
+      </c>
+      <c r="I253">
+        <v>1</v>
+      </c>
+      <c r="J253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>265</v>
+      </c>
+      <c r="B254">
+        <v>0</v>
+      </c>
+      <c r="C254">
+        <v>0</v>
+      </c>
+      <c r="D254">
+        <v>0</v>
+      </c>
+      <c r="E254">
+        <v>0</v>
+      </c>
+      <c r="F254">
+        <v>0</v>
+      </c>
+      <c r="G254">
+        <v>0</v>
+      </c>
+      <c r="H254">
+        <v>0</v>
+      </c>
+      <c r="I254">
+        <v>1</v>
+      </c>
+      <c r="J254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>70</v>
+      </c>
+      <c r="B255">
+        <v>0</v>
+      </c>
+      <c r="C255">
+        <v>0</v>
+      </c>
+      <c r="D255">
+        <v>0</v>
+      </c>
+      <c r="E255">
+        <v>0</v>
+      </c>
+      <c r="F255">
+        <v>0</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
+      <c r="H255">
+        <v>0</v>
+      </c>
+      <c r="I255">
+        <v>1</v>
+      </c>
+      <c r="J255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>266</v>
+      </c>
+      <c r="B256">
+        <v>0</v>
+      </c>
+      <c r="C256">
+        <v>0</v>
+      </c>
+      <c r="D256">
+        <v>0</v>
+      </c>
+      <c r="E256">
+        <v>0</v>
+      </c>
+      <c r="F256">
+        <v>0</v>
+      </c>
+      <c r="G256">
+        <v>0</v>
+      </c>
+      <c r="H256">
+        <v>0</v>
+      </c>
+      <c r="I256">
+        <v>1</v>
+      </c>
+      <c r="J256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>267</v>
+      </c>
+      <c r="B257">
+        <v>0</v>
+      </c>
+      <c r="C257">
+        <v>0</v>
+      </c>
+      <c r="D257">
+        <v>0</v>
+      </c>
+      <c r="E257">
+        <v>0</v>
+      </c>
+      <c r="F257">
+        <v>0</v>
+      </c>
+      <c r="G257">
+        <v>0</v>
+      </c>
+      <c r="H257">
+        <v>0</v>
+      </c>
+      <c r="I257">
+        <v>0</v>
+      </c>
+      <c r="J257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>268</v>
+      </c>
+      <c r="B258">
+        <v>0</v>
+      </c>
+      <c r="C258">
+        <v>0</v>
+      </c>
+      <c r="D258">
+        <v>0</v>
+      </c>
+      <c r="E258">
+        <v>0</v>
+      </c>
+      <c r="F258">
+        <v>0</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
+      <c r="H258">
+        <v>0</v>
+      </c>
+      <c r="I258">
+        <v>0</v>
+      </c>
+      <c r="J258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>269</v>
+      </c>
+      <c r="B259">
+        <v>0</v>
+      </c>
+      <c r="C259">
+        <v>0</v>
+      </c>
+      <c r="D259">
+        <v>0</v>
+      </c>
+      <c r="E259">
+        <v>0</v>
+      </c>
+      <c r="F259">
+        <v>0</v>
+      </c>
+      <c r="G259">
+        <v>0</v>
+      </c>
+      <c r="H259">
+        <v>0</v>
+      </c>
+      <c r="I259">
+        <v>0</v>
+      </c>
+      <c r="J259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>270</v>
+      </c>
+      <c r="B260">
+        <v>0</v>
+      </c>
+      <c r="C260">
+        <v>0</v>
+      </c>
+      <c r="D260">
+        <v>0</v>
+      </c>
+      <c r="E260">
+        <v>0</v>
+      </c>
+      <c r="F260">
+        <v>0</v>
+      </c>
+      <c r="G260">
+        <v>0</v>
+      </c>
+      <c r="H260">
+        <v>0</v>
+      </c>
+      <c r="I260">
+        <v>0</v>
+      </c>
+      <c r="J260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>271</v>
+      </c>
+      <c r="B261">
+        <v>0</v>
+      </c>
+      <c r="C261">
+        <v>0</v>
+      </c>
+      <c r="D261">
+        <v>0</v>
+      </c>
+      <c r="E261">
+        <v>0</v>
+      </c>
+      <c r="F261">
+        <v>0</v>
+      </c>
+      <c r="G261">
+        <v>0</v>
+      </c>
+      <c r="H261">
+        <v>0</v>
+      </c>
+      <c r="I261">
+        <v>0</v>
+      </c>
+      <c r="J261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>272</v>
+      </c>
+      <c r="B262">
+        <v>0</v>
+      </c>
+      <c r="C262">
+        <v>0</v>
+      </c>
+      <c r="D262">
+        <v>0</v>
+      </c>
+      <c r="E262">
+        <v>0</v>
+      </c>
+      <c r="F262">
+        <v>0</v>
+      </c>
+      <c r="G262">
+        <v>0</v>
+      </c>
+      <c r="H262">
+        <v>0</v>
+      </c>
+      <c r="I262">
+        <v>1</v>
+      </c>
+      <c r="J262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>273</v>
+      </c>
+      <c r="B263">
+        <v>0</v>
+      </c>
+      <c r="C263">
+        <v>0</v>
+      </c>
+      <c r="D263">
+        <v>0</v>
+      </c>
+      <c r="E263">
+        <v>0</v>
+      </c>
+      <c r="F263">
+        <v>0</v>
+      </c>
+      <c r="G263">
+        <v>0</v>
+      </c>
+      <c r="H263">
+        <v>0</v>
+      </c>
+      <c r="I263">
+        <v>1</v>
+      </c>
+      <c r="J263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>274</v>
+      </c>
+      <c r="B264">
+        <v>0</v>
+      </c>
+      <c r="C264">
+        <v>0</v>
+      </c>
+      <c r="D264">
+        <v>0</v>
+      </c>
+      <c r="E264">
+        <v>0</v>
+      </c>
+      <c r="F264">
+        <v>0</v>
+      </c>
+      <c r="G264">
+        <v>0</v>
+      </c>
+      <c r="H264">
+        <v>0</v>
+      </c>
+      <c r="I264">
+        <v>1</v>
+      </c>
+      <c r="J264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>275</v>
+      </c>
+      <c r="B265">
+        <v>0</v>
+      </c>
+      <c r="C265">
+        <v>0</v>
+      </c>
+      <c r="D265">
+        <v>0</v>
+      </c>
+      <c r="E265">
+        <v>0</v>
+      </c>
+      <c r="F265">
+        <v>0</v>
+      </c>
+      <c r="G265">
+        <v>0</v>
+      </c>
+      <c r="H265">
+        <v>0</v>
+      </c>
+      <c r="I265">
+        <v>1</v>
+      </c>
+      <c r="J265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>276</v>
+      </c>
+      <c r="B266">
+        <v>0</v>
+      </c>
+      <c r="C266">
+        <v>0</v>
+      </c>
+      <c r="D266">
+        <v>0</v>
+      </c>
+      <c r="E266">
+        <v>0</v>
+      </c>
+      <c r="F266">
+        <v>0</v>
+      </c>
+      <c r="G266">
+        <v>0</v>
+      </c>
+      <c r="H266">
+        <v>0</v>
+      </c>
+      <c r="I266">
+        <v>1</v>
+      </c>
+      <c r="J266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>277</v>
+      </c>
+      <c r="B267">
+        <v>0</v>
+      </c>
+      <c r="C267">
+        <v>0</v>
+      </c>
+      <c r="D267">
+        <v>0</v>
+      </c>
+      <c r="E267">
+        <v>0</v>
+      </c>
+      <c r="F267">
+        <v>0</v>
+      </c>
+      <c r="G267">
+        <v>0</v>
+      </c>
+      <c r="H267">
+        <v>0</v>
+      </c>
+      <c r="I267">
+        <v>1</v>
+      </c>
+      <c r="J267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>278</v>
+      </c>
+      <c r="B268">
+        <v>0</v>
+      </c>
+      <c r="C268">
+        <v>0</v>
+      </c>
+      <c r="D268">
+        <v>0</v>
+      </c>
+      <c r="E268">
+        <v>0</v>
+      </c>
+      <c r="F268">
+        <v>0</v>
+      </c>
+      <c r="G268">
+        <v>0</v>
+      </c>
+      <c r="H268">
+        <v>0</v>
+      </c>
+      <c r="I268">
+        <v>1</v>
+      </c>
+      <c r="J268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>279</v>
+      </c>
+      <c r="B269">
+        <v>0</v>
+      </c>
+      <c r="C269">
+        <v>0</v>
+      </c>
+      <c r="D269">
+        <v>0</v>
+      </c>
+      <c r="E269">
+        <v>0</v>
+      </c>
+      <c r="F269">
+        <v>0</v>
+      </c>
+      <c r="G269">
+        <v>0</v>
+      </c>
+      <c r="H269">
+        <v>0</v>
+      </c>
+      <c r="I269">
+        <v>1</v>
+      </c>
+      <c r="J269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>280</v>
+      </c>
+      <c r="B270">
+        <v>0</v>
+      </c>
+      <c r="C270">
+        <v>0</v>
+      </c>
+      <c r="D270">
+        <v>0</v>
+      </c>
+      <c r="E270">
+        <v>0</v>
+      </c>
+      <c r="F270">
+        <v>0</v>
+      </c>
+      <c r="G270">
+        <v>0</v>
+      </c>
+      <c r="H270">
+        <v>0</v>
+      </c>
+      <c r="I270">
+        <v>1</v>
+      </c>
+      <c r="J270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>281</v>
+      </c>
+      <c r="B271">
+        <v>0</v>
+      </c>
+      <c r="C271">
+        <v>0</v>
+      </c>
+      <c r="D271">
+        <v>0</v>
+      </c>
+      <c r="E271">
+        <v>0</v>
+      </c>
+      <c r="F271">
+        <v>0</v>
+      </c>
+      <c r="G271">
+        <v>0</v>
+      </c>
+      <c r="H271">
+        <v>0</v>
+      </c>
+      <c r="I271">
+        <v>0</v>
+      </c>
+      <c r="J271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>282</v>
+      </c>
+      <c r="B272">
+        <v>0</v>
+      </c>
+      <c r="C272">
+        <v>0</v>
+      </c>
+      <c r="D272">
+        <v>0</v>
+      </c>
+      <c r="E272">
+        <v>0</v>
+      </c>
+      <c r="F272">
+        <v>0</v>
+      </c>
+      <c r="G272">
+        <v>0</v>
+      </c>
+      <c r="H272">
+        <v>0</v>
+      </c>
+      <c r="I272">
+        <v>1</v>
+      </c>
+      <c r="J272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>283</v>
+      </c>
+      <c r="B273">
+        <v>0</v>
+      </c>
+      <c r="C273">
+        <v>0</v>
+      </c>
+      <c r="D273">
+        <v>0</v>
+      </c>
+      <c r="E273">
+        <v>0</v>
+      </c>
+      <c r="F273">
+        <v>0</v>
+      </c>
+      <c r="G273">
+        <v>0</v>
+      </c>
+      <c r="H273">
+        <v>0</v>
+      </c>
+      <c r="I273">
+        <v>1</v>
+      </c>
+      <c r="J273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>284</v>
+      </c>
+      <c r="B274">
+        <v>0</v>
+      </c>
+      <c r="C274">
+        <v>0</v>
+      </c>
+      <c r="D274">
+        <v>0</v>
+      </c>
+      <c r="E274">
+        <v>0</v>
+      </c>
+      <c r="F274">
+        <v>0</v>
+      </c>
+      <c r="G274">
+        <v>0</v>
+      </c>
+      <c r="H274">
+        <v>0</v>
+      </c>
+      <c r="I274">
+        <v>1</v>
+      </c>
+      <c r="J274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>285</v>
+      </c>
+      <c r="B275">
+        <v>0</v>
+      </c>
+      <c r="C275">
+        <v>0</v>
+      </c>
+      <c r="D275">
+        <v>0</v>
+      </c>
+      <c r="E275">
+        <v>0</v>
+      </c>
+      <c r="F275">
+        <v>0</v>
+      </c>
+      <c r="G275">
+        <v>0</v>
+      </c>
+      <c r="H275">
+        <v>0</v>
+      </c>
+      <c r="I275">
+        <v>1</v>
+      </c>
+      <c r="J275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>286</v>
+      </c>
+      <c r="B276">
+        <v>0</v>
+      </c>
+      <c r="C276">
+        <v>0</v>
+      </c>
+      <c r="D276">
+        <v>0</v>
+      </c>
+      <c r="E276">
+        <v>0</v>
+      </c>
+      <c r="F276">
+        <v>0</v>
+      </c>
+      <c r="G276">
+        <v>0</v>
+      </c>
+      <c r="H276">
+        <v>0</v>
+      </c>
+      <c r="I276">
+        <v>1</v>
+      </c>
+      <c r="J276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>287</v>
+      </c>
+      <c r="B277">
+        <v>0</v>
+      </c>
+      <c r="C277">
+        <v>0</v>
+      </c>
+      <c r="D277">
+        <v>0</v>
+      </c>
+      <c r="E277">
+        <v>0</v>
+      </c>
+      <c r="F277">
+        <v>0</v>
+      </c>
+      <c r="G277">
+        <v>0</v>
+      </c>
+      <c r="H277">
+        <v>0</v>
+      </c>
+      <c r="I277">
+        <v>1</v>
+      </c>
+      <c r="J277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>288</v>
+      </c>
+      <c r="B278">
+        <v>0</v>
+      </c>
+      <c r="C278">
+        <v>0</v>
+      </c>
+      <c r="D278">
+        <v>0</v>
+      </c>
+      <c r="E278">
+        <v>0</v>
+      </c>
+      <c r="F278">
+        <v>0</v>
+      </c>
+      <c r="G278">
+        <v>0</v>
+      </c>
+      <c r="H278">
+        <v>0</v>
+      </c>
+      <c r="I278">
+        <v>1</v>
+      </c>
+      <c r="J278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>289</v>
+      </c>
+      <c r="B279">
+        <v>0</v>
+      </c>
+      <c r="C279">
+        <v>0</v>
+      </c>
+      <c r="D279">
+        <v>0</v>
+      </c>
+      <c r="E279">
+        <v>0</v>
+      </c>
+      <c r="F279">
+        <v>0</v>
+      </c>
+      <c r="G279">
+        <v>0</v>
+      </c>
+      <c r="H279">
+        <v>0</v>
+      </c>
+      <c r="I279">
+        <v>1</v>
+      </c>
+      <c r="J279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>290</v>
+      </c>
+      <c r="B280">
+        <v>0</v>
+      </c>
+      <c r="C280">
+        <v>0</v>
+      </c>
+      <c r="D280">
+        <v>0</v>
+      </c>
+      <c r="E280">
+        <v>0</v>
+      </c>
+      <c r="F280">
+        <v>0</v>
+      </c>
+      <c r="G280">
+        <v>1</v>
+      </c>
+      <c r="H280">
+        <v>0</v>
+      </c>
+      <c r="I280">
+        <v>1</v>
+      </c>
+      <c r="J280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>291</v>
+      </c>
+      <c r="B281">
+        <v>0</v>
+      </c>
+      <c r="C281">
+        <v>0</v>
+      </c>
+      <c r="D281">
+        <v>0</v>
+      </c>
+      <c r="E281">
+        <v>0</v>
+      </c>
+      <c r="F281">
+        <v>0</v>
+      </c>
+      <c r="G281">
+        <v>0</v>
+      </c>
+      <c r="H281">
+        <v>0</v>
+      </c>
+      <c r="I281">
+        <v>1</v>
+      </c>
+      <c r="J281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>292</v>
+      </c>
+      <c r="B282">
+        <v>0</v>
+      </c>
+      <c r="C282">
+        <v>0</v>
+      </c>
+      <c r="D282">
+        <v>0</v>
+      </c>
+      <c r="E282">
+        <v>0</v>
+      </c>
+      <c r="F282">
+        <v>0</v>
+      </c>
+      <c r="G282">
+        <v>0</v>
+      </c>
+      <c r="H282">
+        <v>0</v>
+      </c>
+      <c r="I282">
+        <v>1</v>
+      </c>
+      <c r="J282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>293</v>
+      </c>
+      <c r="B283">
+        <v>0</v>
+      </c>
+      <c r="C283">
+        <v>0</v>
+      </c>
+      <c r="D283">
+        <v>0</v>
+      </c>
+      <c r="E283">
+        <v>0</v>
+      </c>
+      <c r="F283">
+        <v>0</v>
+      </c>
+      <c r="G283">
+        <v>0</v>
+      </c>
+      <c r="H283">
+        <v>0</v>
+      </c>
+      <c r="I283">
+        <v>1</v>
+      </c>
+      <c r="J283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>294</v>
+      </c>
+      <c r="B284">
+        <v>0</v>
+      </c>
+      <c r="C284">
+        <v>0</v>
+      </c>
+      <c r="D284">
+        <v>0</v>
+      </c>
+      <c r="E284">
+        <v>0</v>
+      </c>
+      <c r="F284">
+        <v>0</v>
+      </c>
+      <c r="G284">
+        <v>1</v>
+      </c>
+      <c r="H284">
+        <v>0</v>
+      </c>
+      <c r="I284">
+        <v>1</v>
+      </c>
+      <c r="J284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>295</v>
+      </c>
+      <c r="B285">
+        <v>0</v>
+      </c>
+      <c r="C285">
+        <v>0</v>
+      </c>
+      <c r="D285">
+        <v>0</v>
+      </c>
+      <c r="E285">
+        <v>0</v>
+      </c>
+      <c r="F285">
+        <v>0</v>
+      </c>
+      <c r="G285">
+        <v>1</v>
+      </c>
+      <c r="H285">
+        <v>0</v>
+      </c>
+      <c r="I285">
+        <v>1</v>
+      </c>
+      <c r="J285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>143</v>
+      </c>
+      <c r="B286">
+        <v>0</v>
+      </c>
+      <c r="C286">
+        <v>0</v>
+      </c>
+      <c r="D286">
+        <v>0</v>
+      </c>
+      <c r="E286">
+        <v>0</v>
+      </c>
+      <c r="F286">
+        <v>0</v>
+      </c>
+      <c r="G286">
+        <v>0</v>
+      </c>
+      <c r="H286">
+        <v>0</v>
+      </c>
+      <c r="I286">
+        <v>1</v>
+      </c>
+      <c r="J286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>296</v>
+      </c>
+      <c r="B287">
+        <v>0</v>
+      </c>
+      <c r="C287">
+        <v>0</v>
+      </c>
+      <c r="D287">
+        <v>0</v>
+      </c>
+      <c r="E287">
+        <v>0</v>
+      </c>
+      <c r="F287">
+        <v>1</v>
+      </c>
+      <c r="G287">
+        <v>0</v>
+      </c>
+      <c r="H287">
+        <v>0</v>
+      </c>
+      <c r="I287">
+        <v>1</v>
+      </c>
+      <c r="J287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>144</v>
+      </c>
+      <c r="B288">
+        <v>0</v>
+      </c>
+      <c r="C288">
+        <v>0</v>
+      </c>
+      <c r="D288">
+        <v>0</v>
+      </c>
+      <c r="E288">
+        <v>0</v>
+      </c>
+      <c r="F288">
+        <v>0</v>
+      </c>
+      <c r="G288">
+        <v>0</v>
+      </c>
+      <c r="H288">
+        <v>0</v>
+      </c>
+      <c r="I288">
+        <v>1</v>
+      </c>
+      <c r="J288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>297</v>
+      </c>
+      <c r="B289">
+        <v>0</v>
+      </c>
+      <c r="C289">
+        <v>0</v>
+      </c>
+      <c r="D289">
+        <v>0</v>
+      </c>
+      <c r="E289">
+        <v>0</v>
+      </c>
+      <c r="F289">
+        <v>0</v>
+      </c>
+      <c r="G289">
+        <v>0</v>
+      </c>
+      <c r="H289">
+        <v>0</v>
+      </c>
+      <c r="I289">
+        <v>1</v>
+      </c>
+      <c r="J289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>145</v>
+      </c>
+      <c r="B290">
+        <v>0</v>
+      </c>
+      <c r="C290">
+        <v>0</v>
+      </c>
+      <c r="D290">
+        <v>0</v>
+      </c>
+      <c r="E290">
+        <v>0</v>
+      </c>
+      <c r="F290">
+        <v>0</v>
+      </c>
+      <c r="G290">
+        <v>0</v>
+      </c>
+      <c r="H290">
+        <v>0</v>
+      </c>
+      <c r="I290">
+        <v>1</v>
+      </c>
+      <c r="J290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>298</v>
+      </c>
+      <c r="B291">
+        <v>0</v>
+      </c>
+      <c r="C291">
+        <v>0</v>
+      </c>
+      <c r="D291">
+        <v>0</v>
+      </c>
+      <c r="E291">
+        <v>0</v>
+      </c>
+      <c r="F291">
+        <v>0</v>
+      </c>
+      <c r="G291">
+        <v>0</v>
+      </c>
+      <c r="H291">
+        <v>0</v>
+      </c>
+      <c r="I291">
+        <v>1</v>
+      </c>
+      <c r="J291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>299</v>
+      </c>
+      <c r="B292">
+        <v>0</v>
+      </c>
+      <c r="C292">
+        <v>0</v>
+      </c>
+      <c r="D292">
+        <v>0</v>
+      </c>
+      <c r="E292">
+        <v>0</v>
+      </c>
+      <c r="F292">
+        <v>0</v>
+      </c>
+      <c r="G292">
+        <v>0</v>
+      </c>
+      <c r="H292">
+        <v>0</v>
+      </c>
+      <c r="I292">
+        <v>1</v>
+      </c>
+      <c r="J292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>300</v>
+      </c>
+      <c r="B293">
+        <v>0</v>
+      </c>
+      <c r="C293">
+        <v>0</v>
+      </c>
+      <c r="D293">
+        <v>0</v>
+      </c>
+      <c r="E293">
+        <v>0</v>
+      </c>
+      <c r="F293">
+        <v>0</v>
+      </c>
+      <c r="G293">
+        <v>0</v>
+      </c>
+      <c r="H293">
+        <v>0</v>
+      </c>
+      <c r="I293">
+        <v>1</v>
+      </c>
+      <c r="J293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>146</v>
+      </c>
+      <c r="B294">
+        <v>0</v>
+      </c>
+      <c r="C294">
+        <v>0</v>
+      </c>
+      <c r="D294">
+        <v>0</v>
+      </c>
+      <c r="E294">
+        <v>0</v>
+      </c>
+      <c r="F294">
+        <v>0</v>
+      </c>
+      <c r="G294">
+        <v>1</v>
+      </c>
+      <c r="H294">
+        <v>0</v>
+      </c>
+      <c r="I294">
+        <v>1</v>
+      </c>
+      <c r="J294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>301</v>
+      </c>
+      <c r="B295">
+        <v>0</v>
+      </c>
+      <c r="C295">
+        <v>0</v>
+      </c>
+      <c r="D295">
+        <v>0</v>
+      </c>
+      <c r="E295">
+        <v>0</v>
+      </c>
+      <c r="F295">
+        <v>0</v>
+      </c>
+      <c r="G295">
+        <v>1</v>
+      </c>
+      <c r="H295">
+        <v>0</v>
+      </c>
+      <c r="I295">
+        <v>1</v>
+      </c>
+      <c r="J295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>302</v>
+      </c>
+      <c r="B296">
+        <v>0</v>
+      </c>
+      <c r="C296">
+        <v>0</v>
+      </c>
+      <c r="D296">
+        <v>0</v>
+      </c>
+      <c r="E296">
+        <v>0</v>
+      </c>
+      <c r="F296">
+        <v>0</v>
+      </c>
+      <c r="G296">
+        <v>1</v>
+      </c>
+      <c r="H296">
+        <v>0</v>
+      </c>
+      <c r="I296">
+        <v>1</v>
+      </c>
+      <c r="J296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>303</v>
+      </c>
+      <c r="B297">
+        <v>0</v>
+      </c>
+      <c r="C297">
+        <v>0</v>
+      </c>
+      <c r="D297">
+        <v>0</v>
+      </c>
+      <c r="E297">
+        <v>0</v>
+      </c>
+      <c r="F297">
+        <v>0</v>
+      </c>
+      <c r="G297">
+        <v>0</v>
+      </c>
+      <c r="H297">
+        <v>0</v>
+      </c>
+      <c r="I297">
+        <v>1</v>
+      </c>
+      <c r="J297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>304</v>
+      </c>
+      <c r="B298">
+        <v>0</v>
+      </c>
+      <c r="C298">
+        <v>0</v>
+      </c>
+      <c r="D298">
+        <v>0</v>
+      </c>
+      <c r="E298">
+        <v>0</v>
+      </c>
+      <c r="F298">
+        <v>0</v>
+      </c>
+      <c r="G298">
+        <v>0</v>
+      </c>
+      <c r="H298">
+        <v>0</v>
+      </c>
+      <c r="I298">
+        <v>0</v>
+      </c>
+      <c r="J298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>305</v>
+      </c>
+      <c r="B299">
+        <v>0</v>
+      </c>
+      <c r="C299">
+        <v>0</v>
+      </c>
+      <c r="D299">
+        <v>0</v>
+      </c>
+      <c r="E299">
+        <v>0</v>
+      </c>
+      <c r="F299">
+        <v>0</v>
+      </c>
+      <c r="G299">
+        <v>0</v>
+      </c>
+      <c r="H299">
+        <v>0</v>
+      </c>
+      <c r="I299">
+        <v>0</v>
+      </c>
+      <c r="J299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>306</v>
+      </c>
+      <c r="B300">
+        <v>0</v>
+      </c>
+      <c r="C300">
+        <v>0</v>
+      </c>
+      <c r="D300">
+        <v>0</v>
+      </c>
+      <c r="E300">
+        <v>0</v>
+      </c>
+      <c r="F300">
+        <v>0</v>
+      </c>
+      <c r="G300">
+        <v>0</v>
+      </c>
+      <c r="H300">
+        <v>0</v>
+      </c>
+      <c r="I300">
+        <v>0</v>
+      </c>
+      <c r="J300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>307</v>
+      </c>
+      <c r="B301">
+        <v>0</v>
+      </c>
+      <c r="C301">
+        <v>0</v>
+      </c>
+      <c r="D301">
+        <v>0</v>
+      </c>
+      <c r="E301">
+        <v>0</v>
+      </c>
+      <c r="F301">
+        <v>0</v>
+      </c>
+      <c r="G301">
+        <v>0</v>
+      </c>
+      <c r="H301">
+        <v>0</v>
+      </c>
+      <c r="I301">
+        <v>1</v>
+      </c>
+      <c r="J301">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished both Hash-map and Linked-List folder. Total 363
</commit_message>
<xml_diff>
--- a/John.xlsx
+++ b/John.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d03dc4ea78fd367a/Documents/S. Y. 2021-2022/1st Sem/Senior Thesis/data labeling/Final data labeling/data-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="736" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2012E89B-0EA3-4E8F-AA8F-9008CC1318C9}"/>
+  <xr:revisionPtr revIDLastSave="889" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4502175-08D0-45E4-8088-054714380DEA}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="3705" windowWidth="21600" windowHeight="11385" xr2:uid="{77CB7C1E-B4AD-45B5-9992-3E1454331525}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="363">
   <si>
     <t>Filename</t>
   </si>
@@ -958,6 +958,171 @@
   </si>
   <si>
     <t>linklistbag.py</t>
+  </si>
+  <si>
+    <t>List (2).java</t>
+  </si>
+  <si>
+    <t>List.java</t>
+  </si>
+  <si>
+    <t>lliststack.py</t>
+  </si>
+  <si>
+    <t>Merge_K_SortedLinkedlist.java</t>
+  </si>
+  <si>
+    <t>middle_element.java</t>
+  </si>
+  <si>
+    <t>NewJFrame.java</t>
+  </si>
+  <si>
+    <t>Node (2).js</t>
+  </si>
+  <si>
+    <t>Node.js</t>
+  </si>
+  <si>
+    <t>node.py</t>
+  </si>
+  <si>
+    <t>open_addressing.py</t>
+  </si>
+  <si>
+    <t>queue (2).py</t>
+  </si>
+  <si>
+    <t>queue-using-linked-list.js</t>
+  </si>
+  <si>
+    <t>queue-using-stack.js</t>
+  </si>
+  <si>
+    <t>Queue.java</t>
+  </si>
+  <si>
+    <t>queue.js</t>
+  </si>
+  <si>
+    <t>queue.py</t>
+  </si>
+  <si>
+    <t>Recursion.java</t>
+  </si>
+  <si>
+    <t>reverse_linkedlist.java</t>
+  </si>
+  <si>
+    <t>reversed_linked_list.py</t>
+  </si>
+  <si>
+    <t>simplified-stacks-using-arrays.js</t>
+  </si>
+  <si>
+    <t>singly_linked_list (2).py</t>
+  </si>
+  <si>
+    <t>singly_linked_list (3).py</t>
+  </si>
+  <si>
+    <t>singly_linked_list (4).py</t>
+  </si>
+  <si>
+    <t>singly_linked_list.py</t>
+  </si>
+  <si>
+    <t>singly_linked.py</t>
+  </si>
+  <si>
+    <t>singly-linked-list.js</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (2).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (3).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (4).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (5).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (6).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (7).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (8).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (9).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList (10).java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList.java</t>
+  </si>
+  <si>
+    <t>SinglyLinkedList.js</t>
+  </si>
+  <si>
+    <t>SkipList (2).java</t>
+  </si>
+  <si>
+    <t>SkipList.java</t>
+  </si>
+  <si>
+    <t>SkipListInterface.java</t>
+  </si>
+  <si>
+    <t>SkipListMap.java</t>
+  </si>
+  <si>
+    <t>SkipListNode.java</t>
+  </si>
+  <si>
+    <t>SLLNode.java</t>
+  </si>
+  <si>
+    <t>sorted_linklistbag.py</t>
+  </si>
+  <si>
+    <t>stack-using-array.js</t>
+  </si>
+  <si>
+    <t>stack-using-linked-list.js</t>
+  </si>
+  <si>
+    <t>Stack.java</t>
+  </si>
+  <si>
+    <t>stack.py</t>
+  </si>
+  <si>
+    <t>swapNodes (2).py</t>
+  </si>
+  <si>
+    <t>swapNodes (3).py</t>
+  </si>
+  <si>
+    <t>swapNodes (4).py</t>
+  </si>
+  <si>
+    <t>swapNodes.py</t>
+  </si>
+  <si>
+    <t>test_linked_list.py</t>
+  </si>
+  <si>
+    <t>tree.js</t>
+  </si>
+  <si>
+    <t>Vectors.java</t>
   </si>
 </sst>
 </file>
@@ -1330,11 +1495,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E621E51-50FD-4EF4-866F-BB44D85D3FB2}">
-  <dimension ref="A1:O301"/>
+  <dimension ref="A1:O364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A286" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I301" sqref="I301"/>
+      <pane ySplit="1" topLeftCell="A334" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I364" sqref="I364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10984,7 +11149,7 @@
         <v>0</v>
       </c>
       <c r="G301">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H301">
         <v>0</v>
@@ -10993,6 +11158,2022 @@
         <v>1</v>
       </c>
       <c r="J301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>308</v>
+      </c>
+      <c r="B302">
+        <v>0</v>
+      </c>
+      <c r="C302">
+        <v>0</v>
+      </c>
+      <c r="D302">
+        <v>0</v>
+      </c>
+      <c r="E302">
+        <v>0</v>
+      </c>
+      <c r="F302">
+        <v>0</v>
+      </c>
+      <c r="G302">
+        <v>0</v>
+      </c>
+      <c r="H302">
+        <v>0</v>
+      </c>
+      <c r="I302">
+        <v>1</v>
+      </c>
+      <c r="J302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>309</v>
+      </c>
+      <c r="B303">
+        <v>0</v>
+      </c>
+      <c r="C303">
+        <v>0</v>
+      </c>
+      <c r="D303">
+        <v>0</v>
+      </c>
+      <c r="E303">
+        <v>0</v>
+      </c>
+      <c r="F303">
+        <v>0</v>
+      </c>
+      <c r="G303">
+        <v>0</v>
+      </c>
+      <c r="H303">
+        <v>0</v>
+      </c>
+      <c r="I303">
+        <v>0</v>
+      </c>
+      <c r="J303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>310</v>
+      </c>
+      <c r="B304">
+        <v>0</v>
+      </c>
+      <c r="C304">
+        <v>0</v>
+      </c>
+      <c r="D304">
+        <v>0</v>
+      </c>
+      <c r="E304">
+        <v>0</v>
+      </c>
+      <c r="F304">
+        <v>0</v>
+      </c>
+      <c r="G304">
+        <v>0</v>
+      </c>
+      <c r="H304">
+        <v>0</v>
+      </c>
+      <c r="I304">
+        <v>1</v>
+      </c>
+      <c r="J304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>149</v>
+      </c>
+      <c r="B305">
+        <v>0</v>
+      </c>
+      <c r="C305">
+        <v>0</v>
+      </c>
+      <c r="D305">
+        <v>0</v>
+      </c>
+      <c r="E305">
+        <v>0</v>
+      </c>
+      <c r="F305">
+        <v>0</v>
+      </c>
+      <c r="G305">
+        <v>0</v>
+      </c>
+      <c r="H305">
+        <v>0</v>
+      </c>
+      <c r="I305">
+        <v>0</v>
+      </c>
+      <c r="J305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>150</v>
+      </c>
+      <c r="B306">
+        <v>0</v>
+      </c>
+      <c r="C306">
+        <v>0</v>
+      </c>
+      <c r="D306">
+        <v>0</v>
+      </c>
+      <c r="E306">
+        <v>0</v>
+      </c>
+      <c r="F306">
+        <v>0</v>
+      </c>
+      <c r="G306">
+        <v>0</v>
+      </c>
+      <c r="H306">
+        <v>0</v>
+      </c>
+      <c r="I306">
+        <v>0</v>
+      </c>
+      <c r="J306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>151</v>
+      </c>
+      <c r="B307">
+        <v>0</v>
+      </c>
+      <c r="C307">
+        <v>0</v>
+      </c>
+      <c r="D307">
+        <v>0</v>
+      </c>
+      <c r="E307">
+        <v>0</v>
+      </c>
+      <c r="F307">
+        <v>0</v>
+      </c>
+      <c r="G307">
+        <v>0</v>
+      </c>
+      <c r="H307">
+        <v>0</v>
+      </c>
+      <c r="I307">
+        <v>0</v>
+      </c>
+      <c r="J307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>152</v>
+      </c>
+      <c r="B308">
+        <v>0</v>
+      </c>
+      <c r="C308">
+        <v>0</v>
+      </c>
+      <c r="D308">
+        <v>0</v>
+      </c>
+      <c r="E308">
+        <v>0</v>
+      </c>
+      <c r="F308">
+        <v>0</v>
+      </c>
+      <c r="G308">
+        <v>0</v>
+      </c>
+      <c r="H308">
+        <v>0</v>
+      </c>
+      <c r="I308">
+        <v>0</v>
+      </c>
+      <c r="J308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>153</v>
+      </c>
+      <c r="B309">
+        <v>0</v>
+      </c>
+      <c r="C309">
+        <v>0</v>
+      </c>
+      <c r="D309">
+        <v>0</v>
+      </c>
+      <c r="E309">
+        <v>0</v>
+      </c>
+      <c r="F309">
+        <v>0</v>
+      </c>
+      <c r="G309">
+        <v>0</v>
+      </c>
+      <c r="H309">
+        <v>0</v>
+      </c>
+      <c r="I309">
+        <v>0</v>
+      </c>
+      <c r="J309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>159</v>
+      </c>
+      <c r="B310">
+        <v>0</v>
+      </c>
+      <c r="C310">
+        <v>0</v>
+      </c>
+      <c r="D310">
+        <v>0</v>
+      </c>
+      <c r="E310">
+        <v>0</v>
+      </c>
+      <c r="F310">
+        <v>0</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
+      </c>
+      <c r="H310">
+        <v>0</v>
+      </c>
+      <c r="I310">
+        <v>0</v>
+      </c>
+      <c r="J310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>311</v>
+      </c>
+      <c r="B311">
+        <v>0</v>
+      </c>
+      <c r="C311">
+        <v>0</v>
+      </c>
+      <c r="D311">
+        <v>0</v>
+      </c>
+      <c r="E311">
+        <v>0</v>
+      </c>
+      <c r="F311">
+        <v>0</v>
+      </c>
+      <c r="G311">
+        <v>0</v>
+      </c>
+      <c r="H311">
+        <v>0</v>
+      </c>
+      <c r="I311">
+        <v>0</v>
+      </c>
+      <c r="J311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>312</v>
+      </c>
+      <c r="B312">
+        <v>0</v>
+      </c>
+      <c r="C312">
+        <v>0</v>
+      </c>
+      <c r="D312">
+        <v>0</v>
+      </c>
+      <c r="E312">
+        <v>0</v>
+      </c>
+      <c r="F312">
+        <v>0</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+      <c r="H312">
+        <v>0</v>
+      </c>
+      <c r="I312">
+        <v>1</v>
+      </c>
+      <c r="J312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>313</v>
+      </c>
+      <c r="B313">
+        <v>0</v>
+      </c>
+      <c r="C313">
+        <v>0</v>
+      </c>
+      <c r="D313">
+        <v>0</v>
+      </c>
+      <c r="E313">
+        <v>0</v>
+      </c>
+      <c r="F313">
+        <v>0</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
+      </c>
+      <c r="H313">
+        <v>0</v>
+      </c>
+      <c r="I313">
+        <v>0</v>
+      </c>
+      <c r="J313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>181</v>
+      </c>
+      <c r="B314">
+        <v>0</v>
+      </c>
+      <c r="C314">
+        <v>0</v>
+      </c>
+      <c r="D314">
+        <v>0</v>
+      </c>
+      <c r="E314">
+        <v>0</v>
+      </c>
+      <c r="F314">
+        <v>0</v>
+      </c>
+      <c r="G314">
+        <v>0</v>
+      </c>
+      <c r="H314">
+        <v>0</v>
+      </c>
+      <c r="I314">
+        <v>0</v>
+      </c>
+      <c r="J314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>314</v>
+      </c>
+      <c r="B315">
+        <v>0</v>
+      </c>
+      <c r="C315">
+        <v>0</v>
+      </c>
+      <c r="D315">
+        <v>0</v>
+      </c>
+      <c r="E315">
+        <v>0</v>
+      </c>
+      <c r="F315">
+        <v>0</v>
+      </c>
+      <c r="G315">
+        <v>0</v>
+      </c>
+      <c r="H315">
+        <v>0</v>
+      </c>
+      <c r="I315">
+        <v>0</v>
+      </c>
+      <c r="J315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>185</v>
+      </c>
+      <c r="B316">
+        <v>0</v>
+      </c>
+      <c r="C316">
+        <v>0</v>
+      </c>
+      <c r="D316">
+        <v>0</v>
+      </c>
+      <c r="E316">
+        <v>0</v>
+      </c>
+      <c r="F316">
+        <v>0</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+      <c r="H316">
+        <v>0</v>
+      </c>
+      <c r="I316">
+        <v>0</v>
+      </c>
+      <c r="J316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>315</v>
+      </c>
+      <c r="B317">
+        <v>0</v>
+      </c>
+      <c r="C317">
+        <v>0</v>
+      </c>
+      <c r="D317">
+        <v>0</v>
+      </c>
+      <c r="E317">
+        <v>0</v>
+      </c>
+      <c r="F317">
+        <v>0</v>
+      </c>
+      <c r="G317">
+        <v>0</v>
+      </c>
+      <c r="H317">
+        <v>0</v>
+      </c>
+      <c r="I317">
+        <v>0</v>
+      </c>
+      <c r="J317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>316</v>
+      </c>
+      <c r="B318">
+        <v>0</v>
+      </c>
+      <c r="C318">
+        <v>0</v>
+      </c>
+      <c r="D318">
+        <v>0</v>
+      </c>
+      <c r="E318">
+        <v>0</v>
+      </c>
+      <c r="F318">
+        <v>0</v>
+      </c>
+      <c r="G318">
+        <v>0</v>
+      </c>
+      <c r="H318">
+        <v>0</v>
+      </c>
+      <c r="I318">
+        <v>0</v>
+      </c>
+      <c r="J318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>317</v>
+      </c>
+      <c r="B319">
+        <v>0</v>
+      </c>
+      <c r="C319">
+        <v>0</v>
+      </c>
+      <c r="D319">
+        <v>0</v>
+      </c>
+      <c r="E319">
+        <v>0</v>
+      </c>
+      <c r="F319">
+        <v>0</v>
+      </c>
+      <c r="G319">
+        <v>1</v>
+      </c>
+      <c r="H319">
+        <v>0</v>
+      </c>
+      <c r="I319">
+        <v>1</v>
+      </c>
+      <c r="J319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>318</v>
+      </c>
+      <c r="B320">
+        <v>0</v>
+      </c>
+      <c r="C320">
+        <v>0</v>
+      </c>
+      <c r="D320">
+        <v>0</v>
+      </c>
+      <c r="E320">
+        <v>0</v>
+      </c>
+      <c r="F320">
+        <v>0</v>
+      </c>
+      <c r="G320">
+        <v>0</v>
+      </c>
+      <c r="H320">
+        <v>0</v>
+      </c>
+      <c r="I320">
+        <v>0</v>
+      </c>
+      <c r="J320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>319</v>
+      </c>
+      <c r="B321">
+        <v>0</v>
+      </c>
+      <c r="C321">
+        <v>0</v>
+      </c>
+      <c r="D321">
+        <v>0</v>
+      </c>
+      <c r="E321">
+        <v>0</v>
+      </c>
+      <c r="F321">
+        <v>0</v>
+      </c>
+      <c r="G321">
+        <v>0</v>
+      </c>
+      <c r="H321">
+        <v>0</v>
+      </c>
+      <c r="I321">
+        <v>0</v>
+      </c>
+      <c r="J321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>320</v>
+      </c>
+      <c r="B322">
+        <v>0</v>
+      </c>
+      <c r="C322">
+        <v>0</v>
+      </c>
+      <c r="D322">
+        <v>0</v>
+      </c>
+      <c r="E322">
+        <v>0</v>
+      </c>
+      <c r="F322">
+        <v>0</v>
+      </c>
+      <c r="G322">
+        <v>0</v>
+      </c>
+      <c r="H322">
+        <v>0</v>
+      </c>
+      <c r="I322">
+        <v>0</v>
+      </c>
+      <c r="J322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>321</v>
+      </c>
+      <c r="B323">
+        <v>0</v>
+      </c>
+      <c r="C323">
+        <v>0</v>
+      </c>
+      <c r="D323">
+        <v>0</v>
+      </c>
+      <c r="E323">
+        <v>0</v>
+      </c>
+      <c r="F323">
+        <v>0</v>
+      </c>
+      <c r="G323">
+        <v>0</v>
+      </c>
+      <c r="H323">
+        <v>0</v>
+      </c>
+      <c r="I323">
+        <v>0</v>
+      </c>
+      <c r="J323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>322</v>
+      </c>
+      <c r="B324">
+        <v>0</v>
+      </c>
+      <c r="C324">
+        <v>0</v>
+      </c>
+      <c r="D324">
+        <v>0</v>
+      </c>
+      <c r="E324">
+        <v>0</v>
+      </c>
+      <c r="F324">
+        <v>0</v>
+      </c>
+      <c r="G324">
+        <v>0</v>
+      </c>
+      <c r="H324">
+        <v>0</v>
+      </c>
+      <c r="I324">
+        <v>0</v>
+      </c>
+      <c r="J324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>323</v>
+      </c>
+      <c r="B325">
+        <v>0</v>
+      </c>
+      <c r="C325">
+        <v>0</v>
+      </c>
+      <c r="D325">
+        <v>0</v>
+      </c>
+      <c r="E325">
+        <v>0</v>
+      </c>
+      <c r="F325">
+        <v>0</v>
+      </c>
+      <c r="G325">
+        <v>0</v>
+      </c>
+      <c r="H325">
+        <v>0</v>
+      </c>
+      <c r="I325">
+        <v>0</v>
+      </c>
+      <c r="J325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>324</v>
+      </c>
+      <c r="B326">
+        <v>0</v>
+      </c>
+      <c r="C326">
+        <v>0</v>
+      </c>
+      <c r="D326">
+        <v>0</v>
+      </c>
+      <c r="E326">
+        <v>0</v>
+      </c>
+      <c r="F326">
+        <v>0</v>
+      </c>
+      <c r="G326">
+        <v>0</v>
+      </c>
+      <c r="H326">
+        <v>0</v>
+      </c>
+      <c r="I326">
+        <v>0</v>
+      </c>
+      <c r="J326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>325</v>
+      </c>
+      <c r="B327">
+        <v>0</v>
+      </c>
+      <c r="C327">
+        <v>0</v>
+      </c>
+      <c r="D327">
+        <v>0</v>
+      </c>
+      <c r="E327">
+        <v>0</v>
+      </c>
+      <c r="F327">
+        <v>0</v>
+      </c>
+      <c r="G327">
+        <v>0</v>
+      </c>
+      <c r="H327">
+        <v>0</v>
+      </c>
+      <c r="I327">
+        <v>1</v>
+      </c>
+      <c r="J327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>326</v>
+      </c>
+      <c r="B328">
+        <v>0</v>
+      </c>
+      <c r="C328">
+        <v>0</v>
+      </c>
+      <c r="D328">
+        <v>0</v>
+      </c>
+      <c r="E328">
+        <v>0</v>
+      </c>
+      <c r="F328">
+        <v>0</v>
+      </c>
+      <c r="G328">
+        <v>0</v>
+      </c>
+      <c r="H328">
+        <v>0</v>
+      </c>
+      <c r="I328">
+        <v>0</v>
+      </c>
+      <c r="J328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>327</v>
+      </c>
+      <c r="B329">
+        <v>0</v>
+      </c>
+      <c r="C329">
+        <v>0</v>
+      </c>
+      <c r="D329">
+        <v>0</v>
+      </c>
+      <c r="E329">
+        <v>0</v>
+      </c>
+      <c r="F329">
+        <v>0</v>
+      </c>
+      <c r="G329">
+        <v>0</v>
+      </c>
+      <c r="H329">
+        <v>0</v>
+      </c>
+      <c r="I329">
+        <v>0</v>
+      </c>
+      <c r="J329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>328</v>
+      </c>
+      <c r="B330">
+        <v>0</v>
+      </c>
+      <c r="C330">
+        <v>0</v>
+      </c>
+      <c r="D330">
+        <v>0</v>
+      </c>
+      <c r="E330">
+        <v>0</v>
+      </c>
+      <c r="F330">
+        <v>0</v>
+      </c>
+      <c r="G330">
+        <v>0</v>
+      </c>
+      <c r="H330">
+        <v>0</v>
+      </c>
+      <c r="I330">
+        <v>1</v>
+      </c>
+      <c r="J330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>329</v>
+      </c>
+      <c r="B331">
+        <v>0</v>
+      </c>
+      <c r="C331">
+        <v>0</v>
+      </c>
+      <c r="D331">
+        <v>0</v>
+      </c>
+      <c r="E331">
+        <v>0</v>
+      </c>
+      <c r="F331">
+        <v>0</v>
+      </c>
+      <c r="G331">
+        <v>0</v>
+      </c>
+      <c r="H331">
+        <v>0</v>
+      </c>
+      <c r="I331">
+        <v>1</v>
+      </c>
+      <c r="J331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>330</v>
+      </c>
+      <c r="B332">
+        <v>0</v>
+      </c>
+      <c r="C332">
+        <v>0</v>
+      </c>
+      <c r="D332">
+        <v>0</v>
+      </c>
+      <c r="E332">
+        <v>0</v>
+      </c>
+      <c r="F332">
+        <v>0</v>
+      </c>
+      <c r="G332">
+        <v>0</v>
+      </c>
+      <c r="H332">
+        <v>0</v>
+      </c>
+      <c r="I332">
+        <v>1</v>
+      </c>
+      <c r="J332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>331</v>
+      </c>
+      <c r="B333">
+        <v>0</v>
+      </c>
+      <c r="C333">
+        <v>0</v>
+      </c>
+      <c r="D333">
+        <v>0</v>
+      </c>
+      <c r="E333">
+        <v>0</v>
+      </c>
+      <c r="F333">
+        <v>0</v>
+      </c>
+      <c r="G333">
+        <v>0</v>
+      </c>
+      <c r="H333">
+        <v>0</v>
+      </c>
+      <c r="I333">
+        <v>1</v>
+      </c>
+      <c r="J333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>332</v>
+      </c>
+      <c r="B334">
+        <v>0</v>
+      </c>
+      <c r="C334">
+        <v>0</v>
+      </c>
+      <c r="D334">
+        <v>0</v>
+      </c>
+      <c r="E334">
+        <v>0</v>
+      </c>
+      <c r="F334">
+        <v>0</v>
+      </c>
+      <c r="G334">
+        <v>1</v>
+      </c>
+      <c r="H334">
+        <v>0</v>
+      </c>
+      <c r="I334">
+        <v>1</v>
+      </c>
+      <c r="J334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>333</v>
+      </c>
+      <c r="B335">
+        <v>0</v>
+      </c>
+      <c r="C335">
+        <v>0</v>
+      </c>
+      <c r="D335">
+        <v>0</v>
+      </c>
+      <c r="E335">
+        <v>0</v>
+      </c>
+      <c r="F335">
+        <v>0</v>
+      </c>
+      <c r="G335">
+        <v>1</v>
+      </c>
+      <c r="H335">
+        <v>0</v>
+      </c>
+      <c r="I335">
+        <v>1</v>
+      </c>
+      <c r="J335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>334</v>
+      </c>
+      <c r="B336">
+        <v>0</v>
+      </c>
+      <c r="C336">
+        <v>0</v>
+      </c>
+      <c r="D336">
+        <v>0</v>
+      </c>
+      <c r="E336">
+        <v>0</v>
+      </c>
+      <c r="F336">
+        <v>0</v>
+      </c>
+      <c r="G336">
+        <v>0</v>
+      </c>
+      <c r="H336">
+        <v>0</v>
+      </c>
+      <c r="I336">
+        <v>1</v>
+      </c>
+      <c r="J336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>335</v>
+      </c>
+      <c r="B337">
+        <v>0</v>
+      </c>
+      <c r="C337">
+        <v>0</v>
+      </c>
+      <c r="D337">
+        <v>0</v>
+      </c>
+      <c r="E337">
+        <v>0</v>
+      </c>
+      <c r="F337">
+        <v>0</v>
+      </c>
+      <c r="G337">
+        <v>0</v>
+      </c>
+      <c r="H337">
+        <v>0</v>
+      </c>
+      <c r="I337">
+        <v>1</v>
+      </c>
+      <c r="J337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>336</v>
+      </c>
+      <c r="B338">
+        <v>0</v>
+      </c>
+      <c r="C338">
+        <v>0</v>
+      </c>
+      <c r="D338">
+        <v>0</v>
+      </c>
+      <c r="E338">
+        <v>0</v>
+      </c>
+      <c r="F338">
+        <v>0</v>
+      </c>
+      <c r="G338">
+        <v>0</v>
+      </c>
+      <c r="H338">
+        <v>0</v>
+      </c>
+      <c r="I338">
+        <v>1</v>
+      </c>
+      <c r="J338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>337</v>
+      </c>
+      <c r="B339">
+        <v>0</v>
+      </c>
+      <c r="C339">
+        <v>0</v>
+      </c>
+      <c r="D339">
+        <v>0</v>
+      </c>
+      <c r="E339">
+        <v>0</v>
+      </c>
+      <c r="F339">
+        <v>0</v>
+      </c>
+      <c r="G339">
+        <v>0</v>
+      </c>
+      <c r="H339">
+        <v>0</v>
+      </c>
+      <c r="I339">
+        <v>1</v>
+      </c>
+      <c r="J339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>338</v>
+      </c>
+      <c r="B340">
+        <v>0</v>
+      </c>
+      <c r="C340">
+        <v>0</v>
+      </c>
+      <c r="D340">
+        <v>0</v>
+      </c>
+      <c r="E340">
+        <v>0</v>
+      </c>
+      <c r="F340">
+        <v>0</v>
+      </c>
+      <c r="G340">
+        <v>0</v>
+      </c>
+      <c r="H340">
+        <v>0</v>
+      </c>
+      <c r="I340">
+        <v>1</v>
+      </c>
+      <c r="J340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>339</v>
+      </c>
+      <c r="B341">
+        <v>0</v>
+      </c>
+      <c r="C341">
+        <v>0</v>
+      </c>
+      <c r="D341">
+        <v>0</v>
+      </c>
+      <c r="E341">
+        <v>0</v>
+      </c>
+      <c r="F341">
+        <v>0</v>
+      </c>
+      <c r="G341">
+        <v>0</v>
+      </c>
+      <c r="H341">
+        <v>0</v>
+      </c>
+      <c r="I341">
+        <v>1</v>
+      </c>
+      <c r="J341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>340</v>
+      </c>
+      <c r="B342">
+        <v>0</v>
+      </c>
+      <c r="C342">
+        <v>0</v>
+      </c>
+      <c r="D342">
+        <v>0</v>
+      </c>
+      <c r="E342">
+        <v>0</v>
+      </c>
+      <c r="F342">
+        <v>0</v>
+      </c>
+      <c r="G342">
+        <v>0</v>
+      </c>
+      <c r="H342">
+        <v>0</v>
+      </c>
+      <c r="I342">
+        <v>1</v>
+      </c>
+      <c r="J342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>341</v>
+      </c>
+      <c r="B343">
+        <v>0</v>
+      </c>
+      <c r="C343">
+        <v>0</v>
+      </c>
+      <c r="D343">
+        <v>0</v>
+      </c>
+      <c r="E343">
+        <v>0</v>
+      </c>
+      <c r="F343">
+        <v>0</v>
+      </c>
+      <c r="G343">
+        <v>1</v>
+      </c>
+      <c r="H343">
+        <v>0</v>
+      </c>
+      <c r="I343">
+        <v>1</v>
+      </c>
+      <c r="J343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>342</v>
+      </c>
+      <c r="B344">
+        <v>0</v>
+      </c>
+      <c r="C344">
+        <v>0</v>
+      </c>
+      <c r="D344">
+        <v>0</v>
+      </c>
+      <c r="E344">
+        <v>0</v>
+      </c>
+      <c r="F344">
+        <v>0</v>
+      </c>
+      <c r="G344">
+        <v>0</v>
+      </c>
+      <c r="H344">
+        <v>0</v>
+      </c>
+      <c r="I344">
+        <v>1</v>
+      </c>
+      <c r="J344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>343</v>
+      </c>
+      <c r="B345">
+        <v>0</v>
+      </c>
+      <c r="C345">
+        <v>0</v>
+      </c>
+      <c r="D345">
+        <v>0</v>
+      </c>
+      <c r="E345">
+        <v>0</v>
+      </c>
+      <c r="F345">
+        <v>0</v>
+      </c>
+      <c r="G345">
+        <v>0</v>
+      </c>
+      <c r="H345">
+        <v>0</v>
+      </c>
+      <c r="I345">
+        <v>1</v>
+      </c>
+      <c r="J345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>344</v>
+      </c>
+      <c r="B346">
+        <v>0</v>
+      </c>
+      <c r="C346">
+        <v>0</v>
+      </c>
+      <c r="D346">
+        <v>0</v>
+      </c>
+      <c r="E346">
+        <v>0</v>
+      </c>
+      <c r="F346">
+        <v>0</v>
+      </c>
+      <c r="G346">
+        <v>0</v>
+      </c>
+      <c r="H346">
+        <v>0</v>
+      </c>
+      <c r="I346">
+        <v>1</v>
+      </c>
+      <c r="J346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>345</v>
+      </c>
+      <c r="B347">
+        <v>0</v>
+      </c>
+      <c r="C347">
+        <v>0</v>
+      </c>
+      <c r="D347">
+        <v>0</v>
+      </c>
+      <c r="E347">
+        <v>0</v>
+      </c>
+      <c r="F347">
+        <v>0</v>
+      </c>
+      <c r="G347">
+        <v>0</v>
+      </c>
+      <c r="H347">
+        <v>0</v>
+      </c>
+      <c r="I347">
+        <v>1</v>
+      </c>
+      <c r="J347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>346</v>
+      </c>
+      <c r="B348">
+        <v>0</v>
+      </c>
+      <c r="C348">
+        <v>0</v>
+      </c>
+      <c r="D348">
+        <v>0</v>
+      </c>
+      <c r="E348">
+        <v>0</v>
+      </c>
+      <c r="F348">
+        <v>0</v>
+      </c>
+      <c r="G348">
+        <v>0</v>
+      </c>
+      <c r="H348">
+        <v>0</v>
+      </c>
+      <c r="I348">
+        <v>0</v>
+      </c>
+      <c r="J348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>347</v>
+      </c>
+      <c r="B349">
+        <v>0</v>
+      </c>
+      <c r="C349">
+        <v>0</v>
+      </c>
+      <c r="D349">
+        <v>0</v>
+      </c>
+      <c r="E349">
+        <v>0</v>
+      </c>
+      <c r="F349">
+        <v>0</v>
+      </c>
+      <c r="G349">
+        <v>0</v>
+      </c>
+      <c r="H349">
+        <v>0</v>
+      </c>
+      <c r="I349">
+        <v>0</v>
+      </c>
+      <c r="J349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>348</v>
+      </c>
+      <c r="B350">
+        <v>0</v>
+      </c>
+      <c r="C350">
+        <v>0</v>
+      </c>
+      <c r="D350">
+        <v>0</v>
+      </c>
+      <c r="E350">
+        <v>0</v>
+      </c>
+      <c r="F350">
+        <v>0</v>
+      </c>
+      <c r="G350">
+        <v>0</v>
+      </c>
+      <c r="H350">
+        <v>0</v>
+      </c>
+      <c r="I350">
+        <v>0</v>
+      </c>
+      <c r="J350">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>349</v>
+      </c>
+      <c r="B351">
+        <v>0</v>
+      </c>
+      <c r="C351">
+        <v>0</v>
+      </c>
+      <c r="D351">
+        <v>0</v>
+      </c>
+      <c r="E351">
+        <v>0</v>
+      </c>
+      <c r="F351">
+        <v>0</v>
+      </c>
+      <c r="G351">
+        <v>0</v>
+      </c>
+      <c r="H351">
+        <v>0</v>
+      </c>
+      <c r="I351">
+        <v>0</v>
+      </c>
+      <c r="J351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>350</v>
+      </c>
+      <c r="B352">
+        <v>0</v>
+      </c>
+      <c r="C352">
+        <v>0</v>
+      </c>
+      <c r="D352">
+        <v>0</v>
+      </c>
+      <c r="E352">
+        <v>0</v>
+      </c>
+      <c r="F352">
+        <v>0</v>
+      </c>
+      <c r="G352">
+        <v>0</v>
+      </c>
+      <c r="H352">
+        <v>0</v>
+      </c>
+      <c r="I352">
+        <v>0</v>
+      </c>
+      <c r="J352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>351</v>
+      </c>
+      <c r="B353">
+        <v>0</v>
+      </c>
+      <c r="C353">
+        <v>0</v>
+      </c>
+      <c r="D353">
+        <v>0</v>
+      </c>
+      <c r="E353">
+        <v>0</v>
+      </c>
+      <c r="F353">
+        <v>0</v>
+      </c>
+      <c r="G353">
+        <v>0</v>
+      </c>
+      <c r="H353">
+        <v>0</v>
+      </c>
+      <c r="I353">
+        <v>1</v>
+      </c>
+      <c r="J353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>352</v>
+      </c>
+      <c r="B354">
+        <v>0</v>
+      </c>
+      <c r="C354">
+        <v>0</v>
+      </c>
+      <c r="D354">
+        <v>0</v>
+      </c>
+      <c r="E354">
+        <v>0</v>
+      </c>
+      <c r="F354">
+        <v>0</v>
+      </c>
+      <c r="G354">
+        <v>0</v>
+      </c>
+      <c r="H354">
+        <v>0</v>
+      </c>
+      <c r="I354">
+        <v>1</v>
+      </c>
+      <c r="J354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>353</v>
+      </c>
+      <c r="B355">
+        <v>0</v>
+      </c>
+      <c r="C355">
+        <v>0</v>
+      </c>
+      <c r="D355">
+        <v>0</v>
+      </c>
+      <c r="E355">
+        <v>0</v>
+      </c>
+      <c r="F355">
+        <v>0</v>
+      </c>
+      <c r="G355">
+        <v>0</v>
+      </c>
+      <c r="H355">
+        <v>0</v>
+      </c>
+      <c r="I355">
+        <v>1</v>
+      </c>
+      <c r="J355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>354</v>
+      </c>
+      <c r="B356">
+        <v>0</v>
+      </c>
+      <c r="C356">
+        <v>0</v>
+      </c>
+      <c r="D356">
+        <v>0</v>
+      </c>
+      <c r="E356">
+        <v>0</v>
+      </c>
+      <c r="F356">
+        <v>0</v>
+      </c>
+      <c r="G356">
+        <v>0</v>
+      </c>
+      <c r="H356">
+        <v>0</v>
+      </c>
+      <c r="I356">
+        <v>1</v>
+      </c>
+      <c r="J356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>355</v>
+      </c>
+      <c r="B357">
+        <v>0</v>
+      </c>
+      <c r="C357">
+        <v>0</v>
+      </c>
+      <c r="D357">
+        <v>0</v>
+      </c>
+      <c r="E357">
+        <v>0</v>
+      </c>
+      <c r="F357">
+        <v>0</v>
+      </c>
+      <c r="G357">
+        <v>0</v>
+      </c>
+      <c r="H357">
+        <v>0</v>
+      </c>
+      <c r="I357">
+        <v>1</v>
+      </c>
+      <c r="J357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>356</v>
+      </c>
+      <c r="B358">
+        <v>0</v>
+      </c>
+      <c r="C358">
+        <v>0</v>
+      </c>
+      <c r="D358">
+        <v>0</v>
+      </c>
+      <c r="E358">
+        <v>0</v>
+      </c>
+      <c r="F358">
+        <v>0</v>
+      </c>
+      <c r="G358">
+        <v>0</v>
+      </c>
+      <c r="H358">
+        <v>0</v>
+      </c>
+      <c r="I358">
+        <v>1</v>
+      </c>
+      <c r="J358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>357</v>
+      </c>
+      <c r="B359">
+        <v>0</v>
+      </c>
+      <c r="C359">
+        <v>0</v>
+      </c>
+      <c r="D359">
+        <v>0</v>
+      </c>
+      <c r="E359">
+        <v>0</v>
+      </c>
+      <c r="F359">
+        <v>0</v>
+      </c>
+      <c r="G359">
+        <v>0</v>
+      </c>
+      <c r="H359">
+        <v>0</v>
+      </c>
+      <c r="I359">
+        <v>1</v>
+      </c>
+      <c r="J359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>358</v>
+      </c>
+      <c r="B360">
+        <v>0</v>
+      </c>
+      <c r="C360">
+        <v>0</v>
+      </c>
+      <c r="D360">
+        <v>0</v>
+      </c>
+      <c r="E360">
+        <v>0</v>
+      </c>
+      <c r="F360">
+        <v>0</v>
+      </c>
+      <c r="G360">
+        <v>0</v>
+      </c>
+      <c r="H360">
+        <v>0</v>
+      </c>
+      <c r="I360">
+        <v>1</v>
+      </c>
+      <c r="J360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>359</v>
+      </c>
+      <c r="B361">
+        <v>0</v>
+      </c>
+      <c r="C361">
+        <v>0</v>
+      </c>
+      <c r="D361">
+        <v>0</v>
+      </c>
+      <c r="E361">
+        <v>0</v>
+      </c>
+      <c r="F361">
+        <v>0</v>
+      </c>
+      <c r="G361">
+        <v>0</v>
+      </c>
+      <c r="H361">
+        <v>0</v>
+      </c>
+      <c r="I361">
+        <v>1</v>
+      </c>
+      <c r="J361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>360</v>
+      </c>
+      <c r="B362">
+        <v>0</v>
+      </c>
+      <c r="C362">
+        <v>0</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+      <c r="E362">
+        <v>0</v>
+      </c>
+      <c r="F362">
+        <v>0</v>
+      </c>
+      <c r="G362">
+        <v>0</v>
+      </c>
+      <c r="H362">
+        <v>0</v>
+      </c>
+      <c r="I362">
+        <v>0</v>
+      </c>
+      <c r="J362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>361</v>
+      </c>
+      <c r="B363">
+        <v>0</v>
+      </c>
+      <c r="C363">
+        <v>0</v>
+      </c>
+      <c r="D363">
+        <v>0</v>
+      </c>
+      <c r="E363">
+        <v>0</v>
+      </c>
+      <c r="F363">
+        <v>0</v>
+      </c>
+      <c r="G363">
+        <v>0</v>
+      </c>
+      <c r="H363">
+        <v>0</v>
+      </c>
+      <c r="I363">
+        <v>0</v>
+      </c>
+      <c r="J363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>362</v>
+      </c>
+      <c r="B364">
+        <v>0</v>
+      </c>
+      <c r="C364">
+        <v>0</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+      <c r="E364">
+        <v>0</v>
+      </c>
+      <c r="F364">
+        <v>0</v>
+      </c>
+      <c r="G364">
+        <v>0</v>
+      </c>
+      <c r="H364">
+        <v>0</v>
+      </c>
+      <c r="I364">
+        <v>0</v>
+      </c>
+      <c r="J364">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 37 labels. Total 400
</commit_message>
<xml_diff>
--- a/John.xlsx
+++ b/John.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d03dc4ea78fd367a/Documents/S. Y. 2021-2022/1st Sem/Senior Thesis/data labeling/Final data labeling/data-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="889" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4502175-08D0-45E4-8088-054714380DEA}"/>
+  <xr:revisionPtr revIDLastSave="972" documentId="8_{571BA2EA-4107-469E-BA47-9C5166929452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{924FE123-40A7-42A9-B64C-F1F6C9800087}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="3705" windowWidth="21600" windowHeight="11385" xr2:uid="{77CB7C1E-B4AD-45B5-9992-3E1454331525}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="400">
   <si>
     <t>Filename</t>
   </si>
@@ -1123,6 +1123,117 @@
   </si>
   <si>
     <t>Vectors.java</t>
+  </si>
+  <si>
+    <t>AVL.py</t>
+  </si>
+  <si>
+    <t>AVLTree.java</t>
+  </si>
+  <si>
+    <t>BestFirstSearch.java</t>
+  </si>
+  <si>
+    <t>bin_search.py</t>
+  </si>
+  <si>
+    <t>Binary Search.java</t>
+  </si>
+  <si>
+    <t>Binary_Search (2).java</t>
+  </si>
+  <si>
+    <t>binary_search (2).py</t>
+  </si>
+  <si>
+    <t>binary_search (3).py</t>
+  </si>
+  <si>
+    <t>binary_search (4).py</t>
+  </si>
+  <si>
+    <t>binary_search (5).py</t>
+  </si>
+  <si>
+    <t>binary_search (6).py</t>
+  </si>
+  <si>
+    <t>binary_search (7).py</t>
+  </si>
+  <si>
+    <t>binary_search (8).py</t>
+  </si>
+  <si>
+    <t>binary_search (9).py</t>
+  </si>
+  <si>
+    <t>binary_search_tree.py</t>
+  </si>
+  <si>
+    <t>Binary_search.java</t>
+  </si>
+  <si>
+    <t>binary_search.py</t>
+  </si>
+  <si>
+    <t>binary-search-tree.js</t>
+  </si>
+  <si>
+    <t>binary.py</t>
+  </si>
+  <si>
+    <t>BinarySearch (2).java</t>
+  </si>
+  <si>
+    <t>BinarySearch (2).js</t>
+  </si>
+  <si>
+    <t>BinarySearch (2).py</t>
+  </si>
+  <si>
+    <t>BinarySearch (3).java</t>
+  </si>
+  <si>
+    <t>BinarySearch (3).js</t>
+  </si>
+  <si>
+    <t>binarySearch (3).py</t>
+  </si>
+  <si>
+    <t>BinarySearch (4).java</t>
+  </si>
+  <si>
+    <t>binarySearch (4).js</t>
+  </si>
+  <si>
+    <t>BinarySearch (5).java</t>
+  </si>
+  <si>
+    <t>BinarySearch (5).js</t>
+  </si>
+  <si>
+    <t>BinarySearch (6).java</t>
+  </si>
+  <si>
+    <t>binarySearch (6).js</t>
+  </si>
+  <si>
+    <t>BinarySearch (7).java</t>
+  </si>
+  <si>
+    <t>binarySearch (7).js</t>
+  </si>
+  <si>
+    <t>BinarySearch (8).java</t>
+  </si>
+  <si>
+    <t>BinarySearch (9).java</t>
+  </si>
+  <si>
+    <t>binarySearch (10).java</t>
+  </si>
+  <si>
+    <t>BinarySearch (11).java</t>
   </si>
 </sst>
 </file>
@@ -1495,11 +1606,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E621E51-50FD-4EF4-866F-BB44D85D3FB2}">
-  <dimension ref="A1:O364"/>
+  <dimension ref="A1:O401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A334" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I364" sqref="I364"/>
+      <pane ySplit="1" topLeftCell="A385" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A402" sqref="A402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13177,6 +13288,1190 @@
         <v>0</v>
       </c>
     </row>
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>363</v>
+      </c>
+      <c r="B365">
+        <v>0</v>
+      </c>
+      <c r="C365">
+        <v>0</v>
+      </c>
+      <c r="D365">
+        <v>0</v>
+      </c>
+      <c r="E365">
+        <v>0</v>
+      </c>
+      <c r="F365">
+        <v>0</v>
+      </c>
+      <c r="G365">
+        <v>0</v>
+      </c>
+      <c r="H365">
+        <v>0</v>
+      </c>
+      <c r="I365">
+        <v>0</v>
+      </c>
+      <c r="J365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>364</v>
+      </c>
+      <c r="B366">
+        <v>0</v>
+      </c>
+      <c r="C366">
+        <v>0</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+      <c r="E366">
+        <v>0</v>
+      </c>
+      <c r="F366">
+        <v>0</v>
+      </c>
+      <c r="G366">
+        <v>0</v>
+      </c>
+      <c r="H366">
+        <v>0</v>
+      </c>
+      <c r="I366">
+        <v>0</v>
+      </c>
+      <c r="J366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>365</v>
+      </c>
+      <c r="B367">
+        <v>0</v>
+      </c>
+      <c r="C367">
+        <v>0</v>
+      </c>
+      <c r="D367">
+        <v>0</v>
+      </c>
+      <c r="E367">
+        <v>0</v>
+      </c>
+      <c r="F367">
+        <v>0</v>
+      </c>
+      <c r="G367">
+        <v>0</v>
+      </c>
+      <c r="H367">
+        <v>0</v>
+      </c>
+      <c r="I367">
+        <v>0</v>
+      </c>
+      <c r="J367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>366</v>
+      </c>
+      <c r="B368">
+        <v>0</v>
+      </c>
+      <c r="C368">
+        <v>0</v>
+      </c>
+      <c r="D368">
+        <v>0</v>
+      </c>
+      <c r="E368">
+        <v>0</v>
+      </c>
+      <c r="F368">
+        <v>0</v>
+      </c>
+      <c r="G368">
+        <v>0</v>
+      </c>
+      <c r="H368">
+        <v>1</v>
+      </c>
+      <c r="I368">
+        <v>0</v>
+      </c>
+      <c r="J368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>367</v>
+      </c>
+      <c r="B369">
+        <v>0</v>
+      </c>
+      <c r="C369">
+        <v>0</v>
+      </c>
+      <c r="D369">
+        <v>0</v>
+      </c>
+      <c r="E369">
+        <v>0</v>
+      </c>
+      <c r="F369">
+        <v>0</v>
+      </c>
+      <c r="G369">
+        <v>0</v>
+      </c>
+      <c r="H369">
+        <v>1</v>
+      </c>
+      <c r="I369">
+        <v>0</v>
+      </c>
+      <c r="J369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>368</v>
+      </c>
+      <c r="B370">
+        <v>0</v>
+      </c>
+      <c r="C370">
+        <v>0</v>
+      </c>
+      <c r="D370">
+        <v>0</v>
+      </c>
+      <c r="E370">
+        <v>0</v>
+      </c>
+      <c r="F370">
+        <v>0</v>
+      </c>
+      <c r="G370">
+        <v>0</v>
+      </c>
+      <c r="H370">
+        <v>1</v>
+      </c>
+      <c r="I370">
+        <v>0</v>
+      </c>
+      <c r="J370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>369</v>
+      </c>
+      <c r="B371">
+        <v>0</v>
+      </c>
+      <c r="C371">
+        <v>0</v>
+      </c>
+      <c r="D371">
+        <v>0</v>
+      </c>
+      <c r="E371">
+        <v>0</v>
+      </c>
+      <c r="F371">
+        <v>0</v>
+      </c>
+      <c r="G371">
+        <v>0</v>
+      </c>
+      <c r="H371">
+        <v>1</v>
+      </c>
+      <c r="I371">
+        <v>0</v>
+      </c>
+      <c r="J371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>370</v>
+      </c>
+      <c r="B372">
+        <v>0</v>
+      </c>
+      <c r="C372">
+        <v>0</v>
+      </c>
+      <c r="D372">
+        <v>0</v>
+      </c>
+      <c r="E372">
+        <v>0</v>
+      </c>
+      <c r="F372">
+        <v>0</v>
+      </c>
+      <c r="G372">
+        <v>0</v>
+      </c>
+      <c r="H372">
+        <v>0</v>
+      </c>
+      <c r="I372">
+        <v>0</v>
+      </c>
+      <c r="J372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>371</v>
+      </c>
+      <c r="B373">
+        <v>0</v>
+      </c>
+      <c r="C373">
+        <v>0</v>
+      </c>
+      <c r="D373">
+        <v>0</v>
+      </c>
+      <c r="E373">
+        <v>0</v>
+      </c>
+      <c r="F373">
+        <v>0</v>
+      </c>
+      <c r="G373">
+        <v>0</v>
+      </c>
+      <c r="H373">
+        <v>1</v>
+      </c>
+      <c r="I373">
+        <v>0</v>
+      </c>
+      <c r="J373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>372</v>
+      </c>
+      <c r="B374">
+        <v>0</v>
+      </c>
+      <c r="C374">
+        <v>0</v>
+      </c>
+      <c r="D374">
+        <v>0</v>
+      </c>
+      <c r="E374">
+        <v>0</v>
+      </c>
+      <c r="F374">
+        <v>0</v>
+      </c>
+      <c r="G374">
+        <v>0</v>
+      </c>
+      <c r="H374">
+        <v>1</v>
+      </c>
+      <c r="I374">
+        <v>0</v>
+      </c>
+      <c r="J374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>373</v>
+      </c>
+      <c r="B375">
+        <v>0</v>
+      </c>
+      <c r="C375">
+        <v>0</v>
+      </c>
+      <c r="D375">
+        <v>0</v>
+      </c>
+      <c r="E375">
+        <v>0</v>
+      </c>
+      <c r="F375">
+        <v>0</v>
+      </c>
+      <c r="G375">
+        <v>0</v>
+      </c>
+      <c r="H375">
+        <v>1</v>
+      </c>
+      <c r="I375">
+        <v>0</v>
+      </c>
+      <c r="J375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>374</v>
+      </c>
+      <c r="B376">
+        <v>0</v>
+      </c>
+      <c r="C376">
+        <v>0</v>
+      </c>
+      <c r="D376">
+        <v>0</v>
+      </c>
+      <c r="E376">
+        <v>0</v>
+      </c>
+      <c r="F376">
+        <v>0</v>
+      </c>
+      <c r="G376">
+        <v>0</v>
+      </c>
+      <c r="H376">
+        <v>1</v>
+      </c>
+      <c r="I376">
+        <v>0</v>
+      </c>
+      <c r="J376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>375</v>
+      </c>
+      <c r="B377">
+        <v>0</v>
+      </c>
+      <c r="C377">
+        <v>0</v>
+      </c>
+      <c r="D377">
+        <v>0</v>
+      </c>
+      <c r="E377">
+        <v>0</v>
+      </c>
+      <c r="F377">
+        <v>0</v>
+      </c>
+      <c r="G377">
+        <v>0</v>
+      </c>
+      <c r="H377">
+        <v>1</v>
+      </c>
+      <c r="I377">
+        <v>0</v>
+      </c>
+      <c r="J377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>376</v>
+      </c>
+      <c r="B378">
+        <v>0</v>
+      </c>
+      <c r="C378">
+        <v>0</v>
+      </c>
+      <c r="D378">
+        <v>0</v>
+      </c>
+      <c r="E378">
+        <v>0</v>
+      </c>
+      <c r="F378">
+        <v>0</v>
+      </c>
+      <c r="G378">
+        <v>0</v>
+      </c>
+      <c r="H378">
+        <v>1</v>
+      </c>
+      <c r="I378">
+        <v>0</v>
+      </c>
+      <c r="J378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>377</v>
+      </c>
+      <c r="B379">
+        <v>0</v>
+      </c>
+      <c r="C379">
+        <v>0</v>
+      </c>
+      <c r="D379">
+        <v>0</v>
+      </c>
+      <c r="E379">
+        <v>0</v>
+      </c>
+      <c r="F379">
+        <v>0</v>
+      </c>
+      <c r="G379">
+        <v>0</v>
+      </c>
+      <c r="H379">
+        <v>0</v>
+      </c>
+      <c r="I379">
+        <v>0</v>
+      </c>
+      <c r="J379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>378</v>
+      </c>
+      <c r="B380">
+        <v>0</v>
+      </c>
+      <c r="C380">
+        <v>0</v>
+      </c>
+      <c r="D380">
+        <v>0</v>
+      </c>
+      <c r="E380">
+        <v>0</v>
+      </c>
+      <c r="F380">
+        <v>0</v>
+      </c>
+      <c r="G380">
+        <v>0</v>
+      </c>
+      <c r="H380">
+        <v>0</v>
+      </c>
+      <c r="I380">
+        <v>0</v>
+      </c>
+      <c r="J380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>379</v>
+      </c>
+      <c r="B381">
+        <v>0</v>
+      </c>
+      <c r="C381">
+        <v>0</v>
+      </c>
+      <c r="D381">
+        <v>0</v>
+      </c>
+      <c r="E381">
+        <v>0</v>
+      </c>
+      <c r="F381">
+        <v>0</v>
+      </c>
+      <c r="G381">
+        <v>0</v>
+      </c>
+      <c r="H381">
+        <v>1</v>
+      </c>
+      <c r="I381">
+        <v>0</v>
+      </c>
+      <c r="J381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>380</v>
+      </c>
+      <c r="B382">
+        <v>0</v>
+      </c>
+      <c r="C382">
+        <v>0</v>
+      </c>
+      <c r="D382">
+        <v>0</v>
+      </c>
+      <c r="E382">
+        <v>0</v>
+      </c>
+      <c r="F382">
+        <v>0</v>
+      </c>
+      <c r="G382">
+        <v>0</v>
+      </c>
+      <c r="H382">
+        <v>0</v>
+      </c>
+      <c r="I382">
+        <v>0</v>
+      </c>
+      <c r="J382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>381</v>
+      </c>
+      <c r="B383">
+        <v>0</v>
+      </c>
+      <c r="C383">
+        <v>0</v>
+      </c>
+      <c r="D383">
+        <v>0</v>
+      </c>
+      <c r="E383">
+        <v>0</v>
+      </c>
+      <c r="F383">
+        <v>0</v>
+      </c>
+      <c r="G383">
+        <v>0</v>
+      </c>
+      <c r="H383">
+        <v>0</v>
+      </c>
+      <c r="I383">
+        <v>0</v>
+      </c>
+      <c r="J383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>382</v>
+      </c>
+      <c r="B384">
+        <v>0</v>
+      </c>
+      <c r="C384">
+        <v>0</v>
+      </c>
+      <c r="D384">
+        <v>0</v>
+      </c>
+      <c r="E384">
+        <v>0</v>
+      </c>
+      <c r="F384">
+        <v>0</v>
+      </c>
+      <c r="G384">
+        <v>0</v>
+      </c>
+      <c r="H384">
+        <v>1</v>
+      </c>
+      <c r="I384">
+        <v>0</v>
+      </c>
+      <c r="J384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>383</v>
+      </c>
+      <c r="B385">
+        <v>0</v>
+      </c>
+      <c r="C385">
+        <v>0</v>
+      </c>
+      <c r="D385">
+        <v>0</v>
+      </c>
+      <c r="E385">
+        <v>0</v>
+      </c>
+      <c r="F385">
+        <v>0</v>
+      </c>
+      <c r="G385">
+        <v>0</v>
+      </c>
+      <c r="H385">
+        <v>1</v>
+      </c>
+      <c r="I385">
+        <v>0</v>
+      </c>
+      <c r="J385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>384</v>
+      </c>
+      <c r="B386">
+        <v>0</v>
+      </c>
+      <c r="C386">
+        <v>0</v>
+      </c>
+      <c r="D386">
+        <v>0</v>
+      </c>
+      <c r="E386">
+        <v>0</v>
+      </c>
+      <c r="F386">
+        <v>0</v>
+      </c>
+      <c r="G386">
+        <v>0</v>
+      </c>
+      <c r="H386">
+        <v>1</v>
+      </c>
+      <c r="I386">
+        <v>0</v>
+      </c>
+      <c r="J386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>385</v>
+      </c>
+      <c r="B387">
+        <v>0</v>
+      </c>
+      <c r="C387">
+        <v>0</v>
+      </c>
+      <c r="D387">
+        <v>0</v>
+      </c>
+      <c r="E387">
+        <v>0</v>
+      </c>
+      <c r="F387">
+        <v>0</v>
+      </c>
+      <c r="G387">
+        <v>0</v>
+      </c>
+      <c r="H387">
+        <v>1</v>
+      </c>
+      <c r="I387">
+        <v>0</v>
+      </c>
+      <c r="J387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>386</v>
+      </c>
+      <c r="B388">
+        <v>0</v>
+      </c>
+      <c r="C388">
+        <v>0</v>
+      </c>
+      <c r="D388">
+        <v>0</v>
+      </c>
+      <c r="E388">
+        <v>0</v>
+      </c>
+      <c r="F388">
+        <v>0</v>
+      </c>
+      <c r="G388">
+        <v>0</v>
+      </c>
+      <c r="H388">
+        <v>1</v>
+      </c>
+      <c r="I388">
+        <v>0</v>
+      </c>
+      <c r="J388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>387</v>
+      </c>
+      <c r="B389">
+        <v>0</v>
+      </c>
+      <c r="C389">
+        <v>0</v>
+      </c>
+      <c r="D389">
+        <v>0</v>
+      </c>
+      <c r="E389">
+        <v>0</v>
+      </c>
+      <c r="F389">
+        <v>0</v>
+      </c>
+      <c r="G389">
+        <v>0</v>
+      </c>
+      <c r="H389">
+        <v>1</v>
+      </c>
+      <c r="I389">
+        <v>0</v>
+      </c>
+      <c r="J389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>388</v>
+      </c>
+      <c r="B390">
+        <v>0</v>
+      </c>
+      <c r="C390">
+        <v>0</v>
+      </c>
+      <c r="D390">
+        <v>0</v>
+      </c>
+      <c r="E390">
+        <v>0</v>
+      </c>
+      <c r="F390">
+        <v>0</v>
+      </c>
+      <c r="G390">
+        <v>0</v>
+      </c>
+      <c r="H390">
+        <v>1</v>
+      </c>
+      <c r="I390">
+        <v>0</v>
+      </c>
+      <c r="J390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>389</v>
+      </c>
+      <c r="B391">
+        <v>0</v>
+      </c>
+      <c r="C391">
+        <v>0</v>
+      </c>
+      <c r="D391">
+        <v>0</v>
+      </c>
+      <c r="E391">
+        <v>0</v>
+      </c>
+      <c r="F391">
+        <v>0</v>
+      </c>
+      <c r="G391">
+        <v>0</v>
+      </c>
+      <c r="H391">
+        <v>1</v>
+      </c>
+      <c r="I391">
+        <v>0</v>
+      </c>
+      <c r="J391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>390</v>
+      </c>
+      <c r="B392">
+        <v>0</v>
+      </c>
+      <c r="C392">
+        <v>0</v>
+      </c>
+      <c r="D392">
+        <v>0</v>
+      </c>
+      <c r="E392">
+        <v>0</v>
+      </c>
+      <c r="F392">
+        <v>0</v>
+      </c>
+      <c r="G392">
+        <v>0</v>
+      </c>
+      <c r="H392">
+        <v>1</v>
+      </c>
+      <c r="I392">
+        <v>0</v>
+      </c>
+      <c r="J392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>391</v>
+      </c>
+      <c r="B393">
+        <v>0</v>
+      </c>
+      <c r="C393">
+        <v>0</v>
+      </c>
+      <c r="D393">
+        <v>0</v>
+      </c>
+      <c r="E393">
+        <v>0</v>
+      </c>
+      <c r="F393">
+        <v>0</v>
+      </c>
+      <c r="G393">
+        <v>0</v>
+      </c>
+      <c r="H393">
+        <v>1</v>
+      </c>
+      <c r="I393">
+        <v>0</v>
+      </c>
+      <c r="J393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>392</v>
+      </c>
+      <c r="B394">
+        <v>0</v>
+      </c>
+      <c r="C394">
+        <v>0</v>
+      </c>
+      <c r="D394">
+        <v>0</v>
+      </c>
+      <c r="E394">
+        <v>0</v>
+      </c>
+      <c r="F394">
+        <v>0</v>
+      </c>
+      <c r="G394">
+        <v>0</v>
+      </c>
+      <c r="H394">
+        <v>1</v>
+      </c>
+      <c r="I394">
+        <v>0</v>
+      </c>
+      <c r="J394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>393</v>
+      </c>
+      <c r="B395">
+        <v>0</v>
+      </c>
+      <c r="C395">
+        <v>0</v>
+      </c>
+      <c r="D395">
+        <v>0</v>
+      </c>
+      <c r="E395">
+        <v>0</v>
+      </c>
+      <c r="F395">
+        <v>0</v>
+      </c>
+      <c r="G395">
+        <v>0</v>
+      </c>
+      <c r="H395">
+        <v>1</v>
+      </c>
+      <c r="I395">
+        <v>0</v>
+      </c>
+      <c r="J395">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>394</v>
+      </c>
+      <c r="B396">
+        <v>0</v>
+      </c>
+      <c r="C396">
+        <v>0</v>
+      </c>
+      <c r="D396">
+        <v>0</v>
+      </c>
+      <c r="E396">
+        <v>0</v>
+      </c>
+      <c r="F396">
+        <v>0</v>
+      </c>
+      <c r="G396">
+        <v>0</v>
+      </c>
+      <c r="H396">
+        <v>1</v>
+      </c>
+      <c r="I396">
+        <v>0</v>
+      </c>
+      <c r="J396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>395</v>
+      </c>
+      <c r="B397">
+        <v>0</v>
+      </c>
+      <c r="C397">
+        <v>0</v>
+      </c>
+      <c r="D397">
+        <v>0</v>
+      </c>
+      <c r="E397">
+        <v>0</v>
+      </c>
+      <c r="F397">
+        <v>0</v>
+      </c>
+      <c r="G397">
+        <v>0</v>
+      </c>
+      <c r="H397">
+        <v>1</v>
+      </c>
+      <c r="I397">
+        <v>0</v>
+      </c>
+      <c r="J397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>396</v>
+      </c>
+      <c r="B398">
+        <v>0</v>
+      </c>
+      <c r="C398">
+        <v>0</v>
+      </c>
+      <c r="D398">
+        <v>0</v>
+      </c>
+      <c r="E398">
+        <v>0</v>
+      </c>
+      <c r="F398">
+        <v>0</v>
+      </c>
+      <c r="G398">
+        <v>0</v>
+      </c>
+      <c r="H398">
+        <v>1</v>
+      </c>
+      <c r="I398">
+        <v>0</v>
+      </c>
+      <c r="J398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>397</v>
+      </c>
+      <c r="B399">
+        <v>0</v>
+      </c>
+      <c r="C399">
+        <v>0</v>
+      </c>
+      <c r="D399">
+        <v>0</v>
+      </c>
+      <c r="E399">
+        <v>0</v>
+      </c>
+      <c r="F399">
+        <v>0</v>
+      </c>
+      <c r="G399">
+        <v>0</v>
+      </c>
+      <c r="H399">
+        <v>1</v>
+      </c>
+      <c r="I399">
+        <v>0</v>
+      </c>
+      <c r="J399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>398</v>
+      </c>
+      <c r="B400">
+        <v>0</v>
+      </c>
+      <c r="C400">
+        <v>0</v>
+      </c>
+      <c r="D400">
+        <v>0</v>
+      </c>
+      <c r="E400">
+        <v>0</v>
+      </c>
+      <c r="F400">
+        <v>1</v>
+      </c>
+      <c r="G400">
+        <v>0</v>
+      </c>
+      <c r="H400">
+        <v>1</v>
+      </c>
+      <c r="I400">
+        <v>0</v>
+      </c>
+      <c r="J400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>399</v>
+      </c>
+      <c r="B401">
+        <v>0</v>
+      </c>
+      <c r="C401">
+        <v>0</v>
+      </c>
+      <c r="D401">
+        <v>0</v>
+      </c>
+      <c r="E401">
+        <v>0</v>
+      </c>
+      <c r="F401">
+        <v>0</v>
+      </c>
+      <c r="G401">
+        <v>0</v>
+      </c>
+      <c r="H401">
+        <v>1</v>
+      </c>
+      <c r="I401">
+        <v>0</v>
+      </c>
+      <c r="J401">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>